<commit_message>
Temporary files to test coverage
</commit_message>
<xml_diff>
--- a/docs/coverage-testing/85b_test_definitions_PIV_ICAM_Test_Cards_Exploded.xlsx
+++ b/docs/coverage-testing/85b_test_definitions_PIV_ICAM_Test_Cards_Exploded.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\docs\coverage-testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08341573-510D-499D-A108-EC96CC612280}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786910F6-6D7C-459C-9ECC-78FC6198CD26}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2775" yWindow="255" windowWidth="25950" windowHeight="15240" tabRatio="634" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2115" uniqueCount="942">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2115" uniqueCount="943">
   <si>
     <t>Test Case</t>
   </si>
@@ -2052,141 +2052,54 @@
     <t>CCC Values of tags present conform to vendor-supplied data</t>
   </si>
   <si>
-    <t>8.1.a</t>
-  </si>
-  <si>
-    <t>8.1.b</t>
-  </si>
-  <si>
-    <t>8.1.c</t>
-  </si>
-  <si>
-    <t>8.1.d</t>
-  </si>
-  <si>
-    <t>8.1.e</t>
-  </si>
-  <si>
-    <t>8.1.f</t>
-  </si>
-  <si>
-    <t>8.1.g</t>
-  </si>
-  <si>
-    <t>8.1.h</t>
-  </si>
-  <si>
-    <t>8.1.i</t>
-  </si>
-  <si>
-    <t>8.1.j</t>
-  </si>
-  <si>
-    <t>8.2.b</t>
-  </si>
-  <si>
-    <t>8.2.c</t>
-  </si>
-  <si>
-    <t>8.2.d</t>
-  </si>
-  <si>
-    <t>8.2.a</t>
-  </si>
-  <si>
-    <t>8.2.e</t>
-  </si>
-  <si>
-    <t>8.2.f</t>
-  </si>
-  <si>
-    <t>8.2.g</t>
-  </si>
-  <si>
-    <t>8.2.h</t>
-  </si>
-  <si>
-    <t>8.2.i</t>
-  </si>
-  <si>
-    <t>8.2.j</t>
-  </si>
-  <si>
-    <t>8.2.k</t>
-  </si>
-  <si>
-    <t>8.2.l</t>
-  </si>
-  <si>
-    <t>8.2.m</t>
-  </si>
-  <si>
-    <t>8.2.n</t>
+    <t>8.2.1</t>
+  </si>
+  <si>
+    <t>8.2.2</t>
+  </si>
+  <si>
+    <t>8.2.3</t>
+  </si>
+  <si>
+    <t>8.2.4</t>
+  </si>
+  <si>
+    <t>8.2.8</t>
+  </si>
+  <si>
+    <t>8.2.5</t>
+  </si>
+  <si>
+    <t>8.1.1</t>
+  </si>
+  <si>
+    <t>8.1.2</t>
+  </si>
+  <si>
+    <t>8.1.3</t>
+  </si>
+  <si>
+    <t>8.1.4</t>
+  </si>
+  <si>
+    <t>8.1.5</t>
+  </si>
+  <si>
+    <t>8.1.6</t>
+  </si>
+  <si>
+    <t>8.1.9</t>
+  </si>
+  <si>
+    <t>8.1.10</t>
   </si>
   <si>
     <t>CHUID_OID:5</t>
   </si>
   <si>
-    <t>8.3.a</t>
-  </si>
-  <si>
-    <t>8.3.b</t>
-  </si>
-  <si>
-    <t>8.3.c</t>
-  </si>
-  <si>
-    <t>8.3.d</t>
-  </si>
-  <si>
-    <t>8.3.e</t>
-  </si>
-  <si>
-    <t>8.3.f</t>
-  </si>
-  <si>
-    <t>8.3.g</t>
-  </si>
-  <si>
-    <t>8.3.h</t>
-  </si>
-  <si>
-    <t>8.3.i</t>
-  </si>
-  <si>
-    <t>8.3.j</t>
-  </si>
-  <si>
     <t>Tag 0xFE has length of 0</t>
   </si>
   <si>
-    <t>8.4.a</t>
-  </si>
-  <si>
-    <t>8.4.b</t>
-  </si>
-  <si>
-    <t>8.4.c</t>
-  </si>
-  <si>
-    <t>8.4.d</t>
-  </si>
-  <si>
-    <t>8.4.e</t>
-  </si>
-  <si>
-    <t>8.4.f</t>
-  </si>
-  <si>
-    <t>8.4.g</t>
-  </si>
-  <si>
-    <t>8.4.h</t>
-  </si>
-  <si>
-    <t>8.4.i</t>
-  </si>
-  <si>
     <t>CHUID of PIV card applet conforms to SP800-73 Appendix A</t>
   </si>
   <si>
@@ -2205,181 +2118,13 @@
     <t>Card Holder Facial Image of PIV card applet conforms to SP800-73 Appendix A</t>
   </si>
   <si>
-    <t>8.5.a</t>
-  </si>
-  <si>
-    <t>8.5.b</t>
-  </si>
-  <si>
-    <t>8.5.c</t>
-  </si>
-  <si>
-    <t>8.5.d</t>
-  </si>
-  <si>
-    <t>8.5.e</t>
-  </si>
-  <si>
-    <t>8.5.f</t>
-  </si>
-  <si>
-    <t>8.5.g</t>
-  </si>
-  <si>
-    <t>8.5.h</t>
-  </si>
-  <si>
-    <t>8.5.i</t>
-  </si>
-  <si>
-    <t>8.5.j</t>
-  </si>
-  <si>
-    <t>8.6.a</t>
-  </si>
-  <si>
     <t xml:space="preserve">Position is one of the valid x,y coordinate types in the original image </t>
   </si>
   <si>
-    <t>8.6.b</t>
-  </si>
-  <si>
-    <t>8.6.c</t>
-  </si>
-  <si>
-    <t>8.6.d</t>
-  </si>
-  <si>
-    <t>8.6.e</t>
-  </si>
-  <si>
-    <t>8.6.f</t>
-  </si>
-  <si>
-    <t>8.6.g</t>
-  </si>
-  <si>
-    <t>8.6.h</t>
-  </si>
-  <si>
-    <t>8.7.b</t>
-  </si>
-  <si>
-    <t>8.7.c</t>
-  </si>
-  <si>
-    <t>8.7.d</t>
-  </si>
-  <si>
-    <t>8.7.e</t>
-  </si>
-  <si>
-    <t>8.7.f</t>
-  </si>
-  <si>
-    <t>8.7.g</t>
-  </si>
-  <si>
-    <t>8.7.h</t>
-  </si>
-  <si>
-    <t>8.7.i</t>
-  </si>
-  <si>
-    <t>8.7.j</t>
-  </si>
-  <si>
-    <t>8.7.a</t>
-  </si>
-  <si>
     <t>X509 Cert for Digital Signature on PIV applet conforms to SP800-73 Appendix A</t>
   </si>
   <si>
-    <t>8.8.b</t>
-  </si>
-  <si>
-    <t>8.8.c</t>
-  </si>
-  <si>
-    <t>8.8.d</t>
-  </si>
-  <si>
-    <t>8.8.e</t>
-  </si>
-  <si>
-    <t>8.8.f</t>
-  </si>
-  <si>
-    <t>8.8.g</t>
-  </si>
-  <si>
-    <t>8.8.h</t>
-  </si>
-  <si>
-    <t>8.8.i</t>
-  </si>
-  <si>
-    <t>8.8.j</t>
-  </si>
-  <si>
-    <t>8.8.a</t>
-  </si>
-  <si>
-    <t>8.9.a</t>
-  </si>
-  <si>
     <t>Confirm that X509 Cert for Card Authentication on PIV applet conforms to SP800-73 Appendix A</t>
-  </si>
-  <si>
-    <t>8.9.b</t>
-  </si>
-  <si>
-    <t>8.9.c</t>
-  </si>
-  <si>
-    <t>8.9.d</t>
-  </si>
-  <si>
-    <t>8.9.e</t>
-  </si>
-  <si>
-    <t>8.9.f</t>
-  </si>
-  <si>
-    <t>8.9.g</t>
-  </si>
-  <si>
-    <t>8.9.h</t>
-  </si>
-  <si>
-    <t>8.9.i</t>
-  </si>
-  <si>
-    <t>8.9.j</t>
-  </si>
-  <si>
-    <t>8.10.a</t>
-  </si>
-  <si>
-    <t>8.10.b</t>
-  </si>
-  <si>
-    <t>8.10.c</t>
-  </si>
-  <si>
-    <t>8.10.d</t>
-  </si>
-  <si>
-    <t>8.10.e</t>
-  </si>
-  <si>
-    <t>8.10.f</t>
-  </si>
-  <si>
-    <t>8.10.g</t>
-  </si>
-  <si>
-    <t>8.10.h</t>
   </si>
   <si>
     <t>SignerId uses ths IssuerAndSerialNumber choice</t>
@@ -2865,6 +2610,264 @@
   </si>
   <si>
     <t>11.1.2.6.3</t>
+  </si>
+  <si>
+    <t>8.1.7</t>
+  </si>
+  <si>
+    <t>8.1.8</t>
+  </si>
+  <si>
+    <t>8.1.11</t>
+  </si>
+  <si>
+    <t>8.2.6</t>
+  </si>
+  <si>
+    <t>8.2.7</t>
+  </si>
+  <si>
+    <t>8.2.9</t>
+  </si>
+  <si>
+    <t>8.2.10</t>
+  </si>
+  <si>
+    <t>8.2.11</t>
+  </si>
+  <si>
+    <t>8.2.12</t>
+  </si>
+  <si>
+    <t>8.2.13</t>
+  </si>
+  <si>
+    <t>8.2.14</t>
+  </si>
+  <si>
+    <t>8.3.1</t>
+  </si>
+  <si>
+    <t>8.3.2</t>
+  </si>
+  <si>
+    <t>8.3.3</t>
+  </si>
+  <si>
+    <t>8.3.4</t>
+  </si>
+  <si>
+    <t>8.3.5</t>
+  </si>
+  <si>
+    <t>8.3.6</t>
+  </si>
+  <si>
+    <t>8.3.7</t>
+  </si>
+  <si>
+    <t>8.3.8</t>
+  </si>
+  <si>
+    <t>8.3.9</t>
+  </si>
+  <si>
+    <t>8.3.10</t>
+  </si>
+  <si>
+    <t>8.4.1</t>
+  </si>
+  <si>
+    <t>8.4.3</t>
+  </si>
+  <si>
+    <t>8.4.4</t>
+  </si>
+  <si>
+    <t>8.4.5</t>
+  </si>
+  <si>
+    <t>8.4.2</t>
+  </si>
+  <si>
+    <t>8.4.6</t>
+  </si>
+  <si>
+    <t>8.4.7</t>
+  </si>
+  <si>
+    <t>8.4.8</t>
+  </si>
+  <si>
+    <t>8.4.9</t>
+  </si>
+  <si>
+    <t>8.5.1</t>
+  </si>
+  <si>
+    <t>8.5.2</t>
+  </si>
+  <si>
+    <t>8.5.3</t>
+  </si>
+  <si>
+    <t>8.5.4</t>
+  </si>
+  <si>
+    <t>8.5.5</t>
+  </si>
+  <si>
+    <t>8.5.6</t>
+  </si>
+  <si>
+    <t>8.5.7</t>
+  </si>
+  <si>
+    <t>8.5.8</t>
+  </si>
+  <si>
+    <t>8.5.9</t>
+  </si>
+  <si>
+    <t>8.5.10</t>
+  </si>
+  <si>
+    <t>8.6.1</t>
+  </si>
+  <si>
+    <t>8.6.2</t>
+  </si>
+  <si>
+    <t>8.6.3</t>
+  </si>
+  <si>
+    <t>8.6.4</t>
+  </si>
+  <si>
+    <t>8.6.5</t>
+  </si>
+  <si>
+    <t>8.6.6</t>
+  </si>
+  <si>
+    <t>8.6.7</t>
+  </si>
+  <si>
+    <t>8.6.8</t>
+  </si>
+  <si>
+    <t>8.7.1</t>
+  </si>
+  <si>
+    <t>8.7.2</t>
+  </si>
+  <si>
+    <t>8.7.3</t>
+  </si>
+  <si>
+    <t>8.7.4</t>
+  </si>
+  <si>
+    <t>8.7.5</t>
+  </si>
+  <si>
+    <t>8.7.6</t>
+  </si>
+  <si>
+    <t>8.7.7</t>
+  </si>
+  <si>
+    <t>8.7.8</t>
+  </si>
+  <si>
+    <t>8.7.9</t>
+  </si>
+  <si>
+    <t>8.7.10</t>
+  </si>
+  <si>
+    <t>8.8.1</t>
+  </si>
+  <si>
+    <t>8.8.2</t>
+  </si>
+  <si>
+    <t>8.8.3</t>
+  </si>
+  <si>
+    <t>8.8.4</t>
+  </si>
+  <si>
+    <t>8.8.5</t>
+  </si>
+  <si>
+    <t>8.8.6</t>
+  </si>
+  <si>
+    <t>8.8.7</t>
+  </si>
+  <si>
+    <t>8.8.8</t>
+  </si>
+  <si>
+    <t>8.8.9</t>
+  </si>
+  <si>
+    <t>8.8.10</t>
+  </si>
+  <si>
+    <t>8.9.1</t>
+  </si>
+  <si>
+    <t>8.9.2</t>
+  </si>
+  <si>
+    <t>8.9.3</t>
+  </si>
+  <si>
+    <t>8.9.4</t>
+  </si>
+  <si>
+    <t>8.9.5</t>
+  </si>
+  <si>
+    <t>8.9.6</t>
+  </si>
+  <si>
+    <t>8.9.7</t>
+  </si>
+  <si>
+    <t>8.9.8</t>
+  </si>
+  <si>
+    <t>8.9.9</t>
+  </si>
+  <si>
+    <t>8.9.10</t>
+  </si>
+  <si>
+    <t>8.10.1</t>
+  </si>
+  <si>
+    <t>8.10.2</t>
+  </si>
+  <si>
+    <t>8.10.3</t>
+  </si>
+  <si>
+    <t>8.10.4</t>
+  </si>
+  <si>
+    <t>8.10.5</t>
+  </si>
+  <si>
+    <t>8.10.6</t>
+  </si>
+  <si>
+    <t>8.10.7</t>
+  </si>
+  <si>
+    <t>8.10.8</t>
   </si>
 </sst>
 </file>
@@ -4107,8 +4110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F254"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D254" sqref="D254"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94:B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4142,10 +4145,10 @@
         <v>128</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>674</v>
+        <v>680</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>720</v>
+        <v>691</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>181</v>
@@ -4159,7 +4162,7 @@
         <v>128</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>675</v>
+        <v>681</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>182</v>
@@ -4173,7 +4176,7 @@
         <v>128</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>676</v>
+        <v>682</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>184</v>
@@ -4187,7 +4190,7 @@
         <v>128</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>677</v>
+        <v>683</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>186</v>
@@ -4201,7 +4204,7 @@
         <v>128</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>678</v>
+        <v>684</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>192</v>
@@ -4215,7 +4218,7 @@
         <v>128</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>679</v>
+        <v>685</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>194</v>
@@ -4229,7 +4232,7 @@
         <v>128</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>680</v>
+        <v>857</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>196</v>
@@ -4243,7 +4246,7 @@
         <v>128</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>681</v>
+        <v>858</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>633</v>
@@ -4257,7 +4260,7 @@
         <v>128</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>682</v>
+        <v>686</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>634</v>
@@ -4271,7 +4274,7 @@
         <v>128</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>683</v>
+        <v>687</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>673</v>
@@ -4285,7 +4288,7 @@
         <v>128</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>681</v>
+        <v>859</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>234</v>
@@ -4299,10 +4302,10 @@
         <v>128</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>687</v>
+        <v>674</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>719</v>
+        <v>690</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>181</v>
@@ -4313,7 +4316,7 @@
         <v>128</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>684</v>
+        <v>675</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>182</v>
@@ -4327,7 +4330,7 @@
         <v>128</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>685</v>
+        <v>676</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>184</v>
@@ -4341,7 +4344,7 @@
         <v>128</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>686</v>
+        <v>677</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>186</v>
@@ -4355,7 +4358,7 @@
         <v>128</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>688</v>
+        <v>679</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>204</v>
@@ -4369,7 +4372,7 @@
         <v>128</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>689</v>
+        <v>860</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>206</v>
@@ -4383,7 +4386,7 @@
         <v>128</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>690</v>
+        <v>861</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>208</v>
@@ -4397,7 +4400,7 @@
         <v>128</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>691</v>
+        <v>678</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>210</v>
@@ -4411,7 +4414,7 @@
         <v>128</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>692</v>
+        <v>862</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>212</v>
@@ -4425,7 +4428,7 @@
         <v>128</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>693</v>
+        <v>863</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>214</v>
@@ -4439,7 +4442,7 @@
         <v>128</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>694</v>
+        <v>864</v>
       </c>
       <c r="C23" t="s">
         <v>216</v>
@@ -4453,7 +4456,7 @@
         <v>128</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>695</v>
+        <v>865</v>
       </c>
       <c r="C24" t="s">
         <v>218</v>
@@ -4467,7 +4470,7 @@
         <v>128</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>696</v>
+        <v>866</v>
       </c>
       <c r="C25" t="s">
         <v>220</v>
@@ -4481,10 +4484,10 @@
         <v>128</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>697</v>
+        <v>867</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>709</v>
+        <v>689</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>233</v>
@@ -4495,10 +4498,10 @@
         <v>128</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>699</v>
+        <v>868</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>721</v>
+        <v>692</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>181</v>
@@ -4509,7 +4512,7 @@
         <v>128</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>700</v>
+        <v>869</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>182</v>
@@ -4523,7 +4526,7 @@
         <v>128</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>701</v>
+        <v>870</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>184</v>
@@ -4537,7 +4540,7 @@
         <v>128</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>702</v>
+        <v>871</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>186</v>
@@ -4551,7 +4554,7 @@
         <v>128</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>703</v>
+        <v>872</v>
       </c>
       <c r="C31" t="s">
         <v>224</v>
@@ -4565,7 +4568,7 @@
         <v>128</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>704</v>
+        <v>873</v>
       </c>
       <c r="C32" t="s">
         <v>226</v>
@@ -4579,7 +4582,7 @@
         <v>128</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>705</v>
+        <v>874</v>
       </c>
       <c r="C33" t="s">
         <v>228</v>
@@ -4593,7 +4596,7 @@
         <v>128</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>706</v>
+        <v>875</v>
       </c>
       <c r="C34" t="s">
         <v>230</v>
@@ -4607,7 +4610,7 @@
         <v>128</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>707</v>
+        <v>876</v>
       </c>
       <c r="C35" t="s">
         <v>232</v>
@@ -4621,10 +4624,10 @@
         <v>128</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>708</v>
+        <v>877</v>
       </c>
       <c r="C36" t="s">
-        <v>709</v>
+        <v>689</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>233</v>
@@ -4635,10 +4638,10 @@
         <v>128</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>710</v>
+        <v>878</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>722</v>
+        <v>693</v>
       </c>
       <c r="D37" s="11" t="s">
         <v>181</v>
@@ -4649,7 +4652,7 @@
         <v>128</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>711</v>
+        <v>882</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>182</v>
@@ -4663,7 +4666,7 @@
         <v>128</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>712</v>
+        <v>879</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>184</v>
@@ -4677,7 +4680,7 @@
         <v>128</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>713</v>
+        <v>880</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>186</v>
@@ -4691,7 +4694,7 @@
         <v>128</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>714</v>
+        <v>881</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>204</v>
@@ -4705,7 +4708,7 @@
         <v>128</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>715</v>
+        <v>883</v>
       </c>
       <c r="C42" s="10" t="s">
         <v>206</v>
@@ -4719,7 +4722,7 @@
         <v>128</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>716</v>
+        <v>884</v>
       </c>
       <c r="C43" s="10" t="s">
         <v>208</v>
@@ -4733,7 +4736,7 @@
         <v>128</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>717</v>
+        <v>885</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>210</v>
@@ -4747,10 +4750,10 @@
         <v>128</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>718</v>
+        <v>886</v>
       </c>
       <c r="C45" t="s">
-        <v>709</v>
+        <v>689</v>
       </c>
       <c r="D45" s="11" t="s">
         <v>233</v>
@@ -4761,10 +4764,10 @@
         <v>128</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>725</v>
+        <v>887</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>723</v>
+        <v>694</v>
       </c>
       <c r="D46" s="11" t="s">
         <v>181</v>
@@ -4775,7 +4778,7 @@
         <v>128</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>726</v>
+        <v>888</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>182</v>
@@ -4789,7 +4792,7 @@
         <v>128</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>727</v>
+        <v>889</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>184</v>
@@ -4803,7 +4806,7 @@
         <v>128</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>728</v>
+        <v>890</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>186</v>
@@ -4817,7 +4820,7 @@
         <v>128</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>729</v>
+        <v>891</v>
       </c>
       <c r="C50" t="s">
         <v>242</v>
@@ -4831,7 +4834,7 @@
         <v>128</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>730</v>
+        <v>892</v>
       </c>
       <c r="C51" t="s">
         <v>244</v>
@@ -4845,7 +4848,7 @@
         <v>128</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>731</v>
+        <v>893</v>
       </c>
       <c r="C52" t="s">
         <v>246</v>
@@ -4859,7 +4862,7 @@
         <v>128</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>732</v>
+        <v>894</v>
       </c>
       <c r="C53" t="s">
         <v>248</v>
@@ -4873,7 +4876,7 @@
         <v>128</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>733</v>
+        <v>895</v>
       </c>
       <c r="C54" t="s">
         <v>250</v>
@@ -4887,10 +4890,10 @@
         <v>128</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>734</v>
+        <v>896</v>
       </c>
       <c r="C55" t="s">
-        <v>709</v>
+        <v>689</v>
       </c>
       <c r="D55" s="11" t="s">
         <v>233</v>
@@ -4901,10 +4904,10 @@
         <v>128</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>735</v>
+        <v>897</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>724</v>
+        <v>695</v>
       </c>
       <c r="D56" s="11" t="s">
         <v>181</v>
@@ -4915,7 +4918,7 @@
         <v>128</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>737</v>
+        <v>898</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>182</v>
@@ -4929,7 +4932,7 @@
         <v>128</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>738</v>
+        <v>899</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>184</v>
@@ -4943,7 +4946,7 @@
         <v>128</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>739</v>
+        <v>900</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>186</v>
@@ -4957,7 +4960,7 @@
         <v>128</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>740</v>
+        <v>901</v>
       </c>
       <c r="C60" t="s">
         <v>252</v>
@@ -4971,10 +4974,10 @@
         <v>128</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>741</v>
+        <v>902</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>736</v>
+        <v>696</v>
       </c>
       <c r="D61" s="11" t="s">
         <v>237</v>
@@ -4985,7 +4988,7 @@
         <v>128</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>742</v>
+        <v>903</v>
       </c>
       <c r="C62" t="s">
         <v>240</v>
@@ -4999,10 +5002,10 @@
         <v>128</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>743</v>
+        <v>904</v>
       </c>
       <c r="C63" t="s">
-        <v>709</v>
+        <v>689</v>
       </c>
       <c r="D63" s="11" t="s">
         <v>233</v>
@@ -5013,10 +5016,10 @@
         <v>128</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>753</v>
+        <v>905</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>754</v>
+        <v>697</v>
       </c>
       <c r="D64" s="11" t="s">
         <v>181</v>
@@ -5030,7 +5033,7 @@
         <v>128</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>744</v>
+        <v>906</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>182</v>
@@ -5044,7 +5047,7 @@
         <v>128</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>745</v>
+        <v>907</v>
       </c>
       <c r="C66" s="6" t="s">
         <v>184</v>
@@ -5058,7 +5061,7 @@
         <v>128</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>746</v>
+        <v>908</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>186</v>
@@ -5072,7 +5075,7 @@
         <v>128</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>747</v>
+        <v>909</v>
       </c>
       <c r="C68" t="s">
         <v>224</v>
@@ -5086,7 +5089,7 @@
         <v>128</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>748</v>
+        <v>910</v>
       </c>
       <c r="C69" t="s">
         <v>226</v>
@@ -5100,7 +5103,7 @@
         <v>128</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>749</v>
+        <v>911</v>
       </c>
       <c r="C70" t="s">
         <v>228</v>
@@ -5114,7 +5117,7 @@
         <v>128</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>750</v>
+        <v>912</v>
       </c>
       <c r="C71" t="s">
         <v>230</v>
@@ -5128,7 +5131,7 @@
         <v>128</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>751</v>
+        <v>913</v>
       </c>
       <c r="C72" t="s">
         <v>232</v>
@@ -5142,10 +5145,10 @@
         <v>128</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>752</v>
+        <v>914</v>
       </c>
       <c r="C73" t="s">
-        <v>709</v>
+        <v>689</v>
       </c>
       <c r="D73" s="11" t="s">
         <v>233</v>
@@ -5156,7 +5159,7 @@
         <v>128</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>764</v>
+        <v>915</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>129</v>
@@ -5173,7 +5176,7 @@
         <v>128</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>755</v>
+        <v>916</v>
       </c>
       <c r="C75" s="6" t="s">
         <v>182</v>
@@ -5187,7 +5190,7 @@
         <v>128</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>756</v>
+        <v>917</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>184</v>
@@ -5201,7 +5204,7 @@
         <v>128</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>757</v>
+        <v>918</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>186</v>
@@ -5215,7 +5218,7 @@
         <v>128</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>758</v>
+        <v>919</v>
       </c>
       <c r="C78" t="s">
         <v>224</v>
@@ -5229,7 +5232,7 @@
         <v>128</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>759</v>
+        <v>920</v>
       </c>
       <c r="C79" t="s">
         <v>226</v>
@@ -5243,7 +5246,7 @@
         <v>128</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>760</v>
+        <v>921</v>
       </c>
       <c r="C80" t="s">
         <v>228</v>
@@ -5257,7 +5260,7 @@
         <v>128</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>761</v>
+        <v>922</v>
       </c>
       <c r="C81" t="s">
         <v>230</v>
@@ -5271,7 +5274,7 @@
         <v>128</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>762</v>
+        <v>923</v>
       </c>
       <c r="C82" t="s">
         <v>232</v>
@@ -5285,10 +5288,10 @@
         <v>128</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>763</v>
+        <v>924</v>
       </c>
       <c r="C83" t="s">
-        <v>709</v>
+        <v>689</v>
       </c>
       <c r="D83" s="11" t="s">
         <v>233</v>
@@ -5299,10 +5302,10 @@
         <v>128</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>765</v>
+        <v>925</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>766</v>
+        <v>698</v>
       </c>
       <c r="D84" s="11" t="s">
         <v>181</v>
@@ -5316,7 +5319,7 @@
         <v>128</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>767</v>
+        <v>926</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>182</v>
@@ -5330,7 +5333,7 @@
         <v>128</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>768</v>
+        <v>927</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>184</v>
@@ -5344,7 +5347,7 @@
         <v>128</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>769</v>
+        <v>928</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>186</v>
@@ -5358,7 +5361,7 @@
         <v>128</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>770</v>
+        <v>929</v>
       </c>
       <c r="C88" t="s">
         <v>224</v>
@@ -5372,7 +5375,7 @@
         <v>128</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>771</v>
+        <v>930</v>
       </c>
       <c r="C89" t="s">
         <v>226</v>
@@ -5386,7 +5389,7 @@
         <v>128</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>772</v>
+        <v>931</v>
       </c>
       <c r="C90" t="s">
         <v>228</v>
@@ -5400,7 +5403,7 @@
         <v>128</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>773</v>
+        <v>932</v>
       </c>
       <c r="C91" t="s">
         <v>230</v>
@@ -5414,7 +5417,7 @@
         <v>128</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>774</v>
+        <v>933</v>
       </c>
       <c r="C92" t="s">
         <v>232</v>
@@ -5428,10 +5431,10 @@
         <v>128</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>775</v>
+        <v>934</v>
       </c>
       <c r="C93" t="s">
-        <v>709</v>
+        <v>689</v>
       </c>
       <c r="D93" s="11" t="s">
         <v>233</v>
@@ -5442,7 +5445,7 @@
         <v>128</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>776</v>
+        <v>935</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>130</v>
@@ -5459,7 +5462,7 @@
         <v>128</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>777</v>
+        <v>936</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>182</v>
@@ -5473,7 +5476,7 @@
         <v>128</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>778</v>
+        <v>937</v>
       </c>
       <c r="C96" s="6" t="s">
         <v>184</v>
@@ -5487,7 +5490,7 @@
         <v>128</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>779</v>
+        <v>938</v>
       </c>
       <c r="C97" s="6" t="s">
         <v>186</v>
@@ -5501,7 +5504,7 @@
         <v>128</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>780</v>
+        <v>939</v>
       </c>
       <c r="C98" t="s">
         <v>254</v>
@@ -5515,7 +5518,7 @@
         <v>128</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>781</v>
+        <v>940</v>
       </c>
       <c r="C99" t="s">
         <v>256</v>
@@ -5529,7 +5532,7 @@
         <v>128</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>782</v>
+        <v>941</v>
       </c>
       <c r="C100" t="s">
         <v>258</v>
@@ -5543,7 +5546,7 @@
         <v>128</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>783</v>
+        <v>942</v>
       </c>
       <c r="C101" t="s">
         <v>260</v>
@@ -6406,7 +6409,7 @@
         <v>128</v>
       </c>
       <c r="B156" s="6" t="s">
-        <v>817</v>
+        <v>732</v>
       </c>
       <c r="C156" s="6" t="s">
         <v>672</v>
@@ -6423,7 +6426,7 @@
         <v>128</v>
       </c>
       <c r="B157" s="6" t="s">
-        <v>818</v>
+        <v>733</v>
       </c>
       <c r="C157" s="6" t="s">
         <v>375</v>
@@ -6437,10 +6440,10 @@
         <v>128</v>
       </c>
       <c r="B158" s="6" t="s">
-        <v>793</v>
+        <v>708</v>
       </c>
       <c r="C158" s="6" t="s">
-        <v>795</v>
+        <v>710</v>
       </c>
       <c r="D158" s="11" t="s">
         <v>330</v>
@@ -6451,10 +6454,10 @@
         <v>128</v>
       </c>
       <c r="B159" s="6" t="s">
-        <v>796</v>
+        <v>711</v>
       </c>
       <c r="C159" s="6" t="s">
-        <v>786</v>
+        <v>701</v>
       </c>
       <c r="D159" s="11" t="s">
         <v>332</v>
@@ -6465,10 +6468,10 @@
         <v>128</v>
       </c>
       <c r="B160" s="6" t="s">
-        <v>811</v>
+        <v>726</v>
       </c>
       <c r="C160" s="6" t="s">
-        <v>791</v>
+        <v>706</v>
       </c>
       <c r="D160" s="11" t="s">
         <v>334</v>
@@ -6479,10 +6482,10 @@
         <v>128</v>
       </c>
       <c r="B161" s="6" t="s">
-        <v>812</v>
+        <v>727</v>
       </c>
       <c r="C161" s="6" t="s">
-        <v>822</v>
+        <v>737</v>
       </c>
       <c r="D161" s="11" t="s">
         <v>336</v>
@@ -6493,10 +6496,10 @@
         <v>128</v>
       </c>
       <c r="B162" s="6" t="s">
-        <v>798</v>
+        <v>713</v>
       </c>
       <c r="C162" s="6" t="s">
-        <v>823</v>
+        <v>738</v>
       </c>
       <c r="D162" s="11" t="s">
         <v>338</v>
@@ -6507,7 +6510,7 @@
         <v>128</v>
       </c>
       <c r="B163" s="6" t="s">
-        <v>799</v>
+        <v>714</v>
       </c>
       <c r="C163" s="6" t="s">
         <v>660</v>
@@ -6521,7 +6524,7 @@
         <v>128</v>
       </c>
       <c r="B164" s="6" t="s">
-        <v>800</v>
+        <v>715</v>
       </c>
       <c r="C164" s="6" t="s">
         <v>661</v>
@@ -6535,10 +6538,10 @@
         <v>128</v>
       </c>
       <c r="B165" s="6" t="s">
-        <v>813</v>
+        <v>728</v>
       </c>
       <c r="C165" s="6" t="s">
-        <v>784</v>
+        <v>699</v>
       </c>
       <c r="D165" s="11" t="s">
         <v>344</v>
@@ -6549,10 +6552,10 @@
         <v>128</v>
       </c>
       <c r="B166" s="6" t="s">
-        <v>814</v>
+        <v>729</v>
       </c>
       <c r="C166" s="6" t="s">
-        <v>785</v>
+        <v>700</v>
       </c>
       <c r="D166" s="11" t="s">
         <v>346</v>
@@ -6563,7 +6566,7 @@
         <v>128</v>
       </c>
       <c r="B167" s="6" t="s">
-        <v>815</v>
+        <v>730</v>
       </c>
       <c r="C167" s="6" t="s">
         <v>663</v>
@@ -6577,10 +6580,10 @@
         <v>128</v>
       </c>
       <c r="B168" s="6" t="s">
-        <v>816</v>
+        <v>731</v>
       </c>
       <c r="C168" s="6" t="s">
-        <v>803</v>
+        <v>718</v>
       </c>
       <c r="D168" s="11" t="s">
         <v>377</v>
@@ -6591,10 +6594,10 @@
         <v>128</v>
       </c>
       <c r="B169" s="6" t="s">
-        <v>801</v>
+        <v>716</v>
       </c>
       <c r="C169" s="6" t="s">
-        <v>788</v>
+        <v>703</v>
       </c>
       <c r="D169" s="11" t="s">
         <v>359</v>
@@ -6605,7 +6608,7 @@
         <v>128</v>
       </c>
       <c r="B170" s="6" t="s">
-        <v>802</v>
+        <v>717</v>
       </c>
       <c r="C170" s="6" t="s">
         <v>664</v>
@@ -6619,10 +6622,10 @@
         <v>128</v>
       </c>
       <c r="B171" s="6" t="s">
-        <v>819</v>
+        <v>734</v>
       </c>
       <c r="C171" s="7" t="s">
-        <v>820</v>
+        <v>735</v>
       </c>
       <c r="D171" s="11" t="s">
         <v>353</v>
@@ -6636,7 +6639,7 @@
         <v>670</v>
       </c>
       <c r="C172" s="6" t="s">
-        <v>787</v>
+        <v>702</v>
       </c>
       <c r="D172" s="11" t="s">
         <v>355</v>
@@ -6647,7 +6650,7 @@
         <v>128</v>
       </c>
       <c r="B173" s="6" t="s">
-        <v>826</v>
+        <v>741</v>
       </c>
       <c r="C173" s="6" t="s">
         <v>358</v>
@@ -6661,7 +6664,7 @@
         <v>128</v>
       </c>
       <c r="B174" s="6" t="s">
-        <v>789</v>
+        <v>704</v>
       </c>
       <c r="C174" s="6" t="s">
         <v>430</v>
@@ -6675,10 +6678,10 @@
         <v>128</v>
       </c>
       <c r="B175" s="6" t="s">
-        <v>871</v>
+        <v>786</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>807</v>
+        <v>722</v>
       </c>
       <c r="D175" s="11" t="s">
         <v>374</v>
@@ -6689,10 +6692,10 @@
         <v>128</v>
       </c>
       <c r="B176" s="6" t="s">
-        <v>872</v>
+        <v>787</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>808</v>
+        <v>723</v>
       </c>
       <c r="D176" s="11" t="s">
         <v>376</v>
@@ -6703,7 +6706,7 @@
         <v>128</v>
       </c>
       <c r="B177" s="6" t="s">
-        <v>873</v>
+        <v>788</v>
       </c>
       <c r="C177" s="4" t="s">
         <v>378</v>
@@ -6717,10 +6720,10 @@
         <v>128</v>
       </c>
       <c r="B178" s="6" t="s">
-        <v>860</v>
+        <v>775</v>
       </c>
       <c r="C178" s="6" t="s">
-        <v>795</v>
+        <v>710</v>
       </c>
       <c r="D178" s="11" t="s">
         <v>330</v>
@@ -6731,10 +6734,10 @@
         <v>128</v>
       </c>
       <c r="B179" s="6" t="s">
-        <v>794</v>
+        <v>709</v>
       </c>
       <c r="C179" s="6" t="s">
-        <v>786</v>
+        <v>701</v>
       </c>
       <c r="D179" s="11" t="s">
         <v>332</v>
@@ -6745,10 +6748,10 @@
         <v>128</v>
       </c>
       <c r="B180" s="6" t="s">
-        <v>861</v>
+        <v>776</v>
       </c>
       <c r="C180" s="6" t="s">
-        <v>791</v>
+        <v>706</v>
       </c>
       <c r="D180" s="11" t="s">
         <v>334</v>
@@ -6759,10 +6762,10 @@
         <v>128</v>
       </c>
       <c r="B181" s="6" t="s">
-        <v>862</v>
+        <v>777</v>
       </c>
       <c r="C181" s="6" t="s">
-        <v>822</v>
+        <v>737</v>
       </c>
       <c r="D181" s="11" t="s">
         <v>336</v>
@@ -6773,10 +6776,10 @@
         <v>128</v>
       </c>
       <c r="B182" s="6" t="s">
-        <v>863</v>
+        <v>778</v>
       </c>
       <c r="C182" s="6" t="s">
-        <v>823</v>
+        <v>738</v>
       </c>
       <c r="D182" s="11" t="s">
         <v>338</v>
@@ -6787,7 +6790,7 @@
         <v>128</v>
       </c>
       <c r="B183" s="6" t="s">
-        <v>797</v>
+        <v>712</v>
       </c>
       <c r="C183" s="6" t="s">
         <v>660</v>
@@ -6801,7 +6804,7 @@
         <v>128</v>
       </c>
       <c r="B184" s="6" t="s">
-        <v>792</v>
+        <v>707</v>
       </c>
       <c r="C184" s="6" t="s">
         <v>661</v>
@@ -6815,10 +6818,10 @@
         <v>128</v>
       </c>
       <c r="B185" s="6" t="s">
-        <v>864</v>
+        <v>779</v>
       </c>
       <c r="C185" s="6" t="s">
-        <v>784</v>
+        <v>699</v>
       </c>
       <c r="D185" s="11" t="s">
         <v>344</v>
@@ -6829,10 +6832,10 @@
         <v>128</v>
       </c>
       <c r="B186" s="6" t="s">
-        <v>865</v>
+        <v>780</v>
       </c>
       <c r="C186" s="6" t="s">
-        <v>785</v>
+        <v>700</v>
       </c>
       <c r="D186" s="11" t="s">
         <v>346</v>
@@ -6843,7 +6846,7 @@
         <v>128</v>
       </c>
       <c r="B187" s="6" t="s">
-        <v>866</v>
+        <v>781</v>
       </c>
       <c r="C187" s="6" t="s">
         <v>663</v>
@@ -6857,10 +6860,10 @@
         <v>128</v>
       </c>
       <c r="B188" s="6" t="s">
-        <v>867</v>
+        <v>782</v>
       </c>
       <c r="C188" s="6" t="s">
-        <v>803</v>
+        <v>718</v>
       </c>
       <c r="D188" s="11" t="s">
         <v>377</v>
@@ -6871,10 +6874,10 @@
         <v>128</v>
       </c>
       <c r="B189" s="6" t="s">
-        <v>790</v>
+        <v>705</v>
       </c>
       <c r="C189" s="6" t="s">
-        <v>788</v>
+        <v>703</v>
       </c>
       <c r="D189" s="11" t="s">
         <v>359</v>
@@ -6885,7 +6888,7 @@
         <v>128</v>
       </c>
       <c r="B190" s="6" t="s">
-        <v>868</v>
+        <v>783</v>
       </c>
       <c r="C190" s="6" t="s">
         <v>664</v>
@@ -6899,10 +6902,10 @@
         <v>128</v>
       </c>
       <c r="B191" s="6" t="s">
-        <v>869</v>
+        <v>784</v>
       </c>
       <c r="C191" s="7" t="s">
-        <v>820</v>
+        <v>735</v>
       </c>
       <c r="D191" s="11" t="s">
         <v>353</v>
@@ -6913,10 +6916,10 @@
         <v>128</v>
       </c>
       <c r="B192" s="6" t="s">
-        <v>874</v>
+        <v>789</v>
       </c>
       <c r="C192" s="6" t="s">
-        <v>787</v>
+        <v>702</v>
       </c>
       <c r="D192" s="11" t="s">
         <v>355</v>
@@ -6927,7 +6930,7 @@
         <v>128</v>
       </c>
       <c r="B193" s="6" t="s">
-        <v>826</v>
+        <v>741</v>
       </c>
       <c r="C193" s="6" t="s">
         <v>358</v>
@@ -6941,7 +6944,7 @@
         <v>128</v>
       </c>
       <c r="B194" s="6" t="s">
-        <v>870</v>
+        <v>785</v>
       </c>
       <c r="C194" s="6" t="s">
         <v>430</v>
@@ -6955,10 +6958,10 @@
         <v>128</v>
       </c>
       <c r="B195" s="6" t="s">
-        <v>885</v>
+        <v>800</v>
       </c>
       <c r="C195" s="6" t="s">
-        <v>886</v>
+        <v>801</v>
       </c>
       <c r="D195" s="11" t="s">
         <v>631</v>
@@ -6975,10 +6978,10 @@
         <v>128</v>
       </c>
       <c r="B196" s="6" t="s">
-        <v>875</v>
+        <v>790</v>
       </c>
       <c r="C196" s="7" t="s">
-        <v>876</v>
+        <v>791</v>
       </c>
       <c r="D196" s="11" t="s">
         <v>330</v>
@@ -6989,7 +6992,7 @@
         <v>128</v>
       </c>
       <c r="B197" s="6" t="s">
-        <v>877</v>
+        <v>792</v>
       </c>
       <c r="C197" s="6" t="s">
         <v>363</v>
@@ -7003,7 +7006,7 @@
         <v>128</v>
       </c>
       <c r="B198" s="6" t="s">
-        <v>879</v>
+        <v>794</v>
       </c>
       <c r="C198" s="6" t="s">
         <v>365</v>
@@ -7017,10 +7020,10 @@
         <v>128</v>
       </c>
       <c r="B199" s="6" t="s">
-        <v>880</v>
+        <v>795</v>
       </c>
       <c r="C199" s="6" t="s">
-        <v>878</v>
+        <v>793</v>
       </c>
       <c r="D199" s="11" t="s">
         <v>366</v>
@@ -7031,10 +7034,10 @@
         <v>128</v>
       </c>
       <c r="B200" s="6" t="s">
-        <v>881</v>
+        <v>796</v>
       </c>
       <c r="C200" s="6" t="s">
-        <v>883</v>
+        <v>798</v>
       </c>
       <c r="D200" s="11" t="s">
         <v>368</v>
@@ -7045,7 +7048,7 @@
         <v>128</v>
       </c>
       <c r="B201" s="6" t="s">
-        <v>882</v>
+        <v>797</v>
       </c>
       <c r="C201" s="6" t="s">
         <v>373</v>
@@ -7059,7 +7062,7 @@
         <v>128</v>
       </c>
       <c r="B202" s="6" t="s">
-        <v>884</v>
+        <v>799</v>
       </c>
       <c r="C202" s="6" t="s">
         <v>667</v>
@@ -7107,10 +7110,10 @@
         <v>128</v>
       </c>
       <c r="B205" s="6" t="s">
-        <v>921</v>
+        <v>836</v>
       </c>
       <c r="C205" s="6" t="s">
-        <v>842</v>
+        <v>757</v>
       </c>
       <c r="D205" s="11" t="s">
         <v>176</v>
@@ -7121,10 +7124,10 @@
         <v>128</v>
       </c>
       <c r="B206" s="6" t="s">
-        <v>920</v>
+        <v>835</v>
       </c>
       <c r="C206" s="6" t="s">
-        <v>843</v>
+        <v>758</v>
       </c>
       <c r="D206" s="17" t="s">
         <v>176</v>
@@ -7135,10 +7138,10 @@
         <v>128</v>
       </c>
       <c r="B207" s="6" t="s">
-        <v>922</v>
+        <v>837</v>
       </c>
       <c r="C207" s="6" t="s">
-        <v>919</v>
+        <v>834</v>
       </c>
       <c r="D207" s="18" t="s">
         <v>176</v>
@@ -7149,10 +7152,10 @@
         <v>128</v>
       </c>
       <c r="B208" s="6" t="s">
-        <v>916</v>
+        <v>831</v>
       </c>
       <c r="C208" s="6" t="s">
-        <v>917</v>
+        <v>832</v>
       </c>
       <c r="D208" s="18" t="s">
         <v>176</v>
@@ -7163,7 +7166,7 @@
         <v>128</v>
       </c>
       <c r="B209" s="6" t="s">
-        <v>918</v>
+        <v>833</v>
       </c>
       <c r="C209" s="6" t="s">
         <v>384</v>
@@ -7177,10 +7180,10 @@
         <v>128</v>
       </c>
       <c r="B210" s="6" t="s">
-        <v>923</v>
+        <v>838</v>
       </c>
       <c r="C210" s="6" t="s">
-        <v>844</v>
+        <v>759</v>
       </c>
       <c r="D210" s="11" t="s">
         <v>385</v>
@@ -7191,7 +7194,7 @@
         <v>128</v>
       </c>
       <c r="B211" s="6" t="s">
-        <v>924</v>
+        <v>839</v>
       </c>
       <c r="C211" s="6" t="s">
         <v>387</v>
@@ -7205,7 +7208,7 @@
         <v>128</v>
       </c>
       <c r="B212" s="6" t="s">
-        <v>925</v>
+        <v>840</v>
       </c>
       <c r="C212" s="6" t="s">
         <v>389</v>
@@ -7219,10 +7222,10 @@
         <v>128</v>
       </c>
       <c r="B213" s="6" t="s">
-        <v>927</v>
+        <v>842</v>
       </c>
       <c r="C213" s="6" t="s">
-        <v>926</v>
+        <v>841</v>
       </c>
       <c r="D213" s="11" t="s">
         <v>390</v>
@@ -7233,10 +7236,10 @@
         <v>128</v>
       </c>
       <c r="B214" s="6" t="s">
-        <v>928</v>
+        <v>843</v>
       </c>
       <c r="C214" s="6" t="s">
-        <v>929</v>
+        <v>844</v>
       </c>
       <c r="D214" s="11" t="s">
         <v>392</v>
@@ -7247,10 +7250,10 @@
         <v>128</v>
       </c>
       <c r="B215" s="6" t="s">
-        <v>931</v>
+        <v>846</v>
       </c>
       <c r="C215" s="6" t="s">
-        <v>930</v>
+        <v>845</v>
       </c>
       <c r="D215" s="11" t="s">
         <v>394</v>
@@ -7261,7 +7264,7 @@
         <v>128</v>
       </c>
       <c r="B216" s="6" t="s">
-        <v>932</v>
+        <v>847</v>
       </c>
       <c r="C216" s="6" t="s">
         <v>397</v>
@@ -7275,7 +7278,7 @@
         <v>128</v>
       </c>
       <c r="B217" s="6" t="s">
-        <v>933</v>
+        <v>848</v>
       </c>
       <c r="C217" s="6" t="s">
         <v>399</v>
@@ -7289,10 +7292,10 @@
         <v>128</v>
       </c>
       <c r="B218" s="6" t="s">
-        <v>934</v>
+        <v>849</v>
       </c>
       <c r="C218" s="6" t="s">
-        <v>936</v>
+        <v>851</v>
       </c>
       <c r="D218" s="11" t="s">
         <v>401</v>
@@ -7303,10 +7306,10 @@
         <v>128</v>
       </c>
       <c r="B219" s="6" t="s">
-        <v>940</v>
+        <v>855</v>
       </c>
       <c r="C219" s="6" t="s">
-        <v>935</v>
+        <v>850</v>
       </c>
       <c r="D219" s="17" t="s">
         <v>401</v>
@@ -7317,10 +7320,10 @@
         <v>128</v>
       </c>
       <c r="B220" s="6" t="s">
-        <v>941</v>
+        <v>856</v>
       </c>
       <c r="C220" s="6" t="s">
-        <v>937</v>
+        <v>852</v>
       </c>
       <c r="D220" s="17" t="s">
         <v>401</v>
@@ -7331,7 +7334,7 @@
         <v>128</v>
       </c>
       <c r="B221" s="6" t="s">
-        <v>938</v>
+        <v>853</v>
       </c>
       <c r="C221" s="6" t="s">
         <v>404</v>
@@ -7345,7 +7348,7 @@
         <v>128</v>
       </c>
       <c r="B222" s="6" t="s">
-        <v>939</v>
+        <v>854</v>
       </c>
       <c r="C222" s="6" t="s">
         <v>406</v>
@@ -7359,10 +7362,10 @@
         <v>128</v>
       </c>
       <c r="B223" s="6" t="s">
-        <v>906</v>
+        <v>821</v>
       </c>
       <c r="C223" s="6" t="s">
-        <v>901</v>
+        <v>816</v>
       </c>
       <c r="D223" s="11" t="s">
         <v>176</v>
@@ -7373,10 +7376,10 @@
         <v>128</v>
       </c>
       <c r="B224" s="6" t="s">
-        <v>907</v>
+        <v>822</v>
       </c>
       <c r="C224" s="6" t="s">
-        <v>849</v>
+        <v>764</v>
       </c>
       <c r="D224" s="17" t="s">
         <v>176</v>
@@ -7388,7 +7391,7 @@
       </c>
       <c r="B225" s="6"/>
       <c r="C225" s="6" t="s">
-        <v>827</v>
+        <v>742</v>
       </c>
       <c r="D225" s="18" t="s">
         <v>381</v>
@@ -7399,10 +7402,10 @@
         <v>128</v>
       </c>
       <c r="B226" s="6" t="s">
-        <v>908</v>
+        <v>823</v>
       </c>
       <c r="C226" s="6" t="s">
-        <v>913</v>
+        <v>828</v>
       </c>
       <c r="D226" s="11" t="s">
         <v>407</v>
@@ -7413,10 +7416,10 @@
         <v>128</v>
       </c>
       <c r="B227" s="6" t="s">
-        <v>909</v>
+        <v>824</v>
       </c>
       <c r="C227" s="6" t="s">
-        <v>902</v>
+        <v>817</v>
       </c>
       <c r="D227" s="11" t="s">
         <v>411</v>
@@ -7427,10 +7430,10 @@
         <v>128</v>
       </c>
       <c r="B228" s="6" t="s">
-        <v>910</v>
+        <v>825</v>
       </c>
       <c r="C228" s="6" t="s">
-        <v>903</v>
+        <v>818</v>
       </c>
       <c r="D228" s="11" t="s">
         <v>385</v>
@@ -7441,10 +7444,10 @@
         <v>128</v>
       </c>
       <c r="B229" s="6" t="s">
-        <v>911</v>
+        <v>826</v>
       </c>
       <c r="C229" s="6" t="s">
-        <v>904</v>
+        <v>819</v>
       </c>
       <c r="D229" s="11" t="s">
         <v>398</v>
@@ -7455,10 +7458,10 @@
         <v>128</v>
       </c>
       <c r="B230" s="6" t="s">
-        <v>912</v>
+        <v>827</v>
       </c>
       <c r="C230" s="6" t="s">
-        <v>915</v>
+        <v>830</v>
       </c>
       <c r="D230" s="11" t="s">
         <v>403</v>
@@ -7469,10 +7472,10 @@
         <v>128</v>
       </c>
       <c r="B231" s="11" t="s">
-        <v>914</v>
+        <v>829</v>
       </c>
       <c r="C231" s="6" t="s">
-        <v>905</v>
+        <v>820</v>
       </c>
       <c r="D231" s="11" t="s">
         <v>405</v>
@@ -7483,10 +7486,10 @@
         <v>128</v>
       </c>
       <c r="B232" s="6" t="s">
-        <v>846</v>
+        <v>761</v>
       </c>
       <c r="C232" s="6" t="s">
-        <v>850</v>
+        <v>765</v>
       </c>
       <c r="D232" s="11" t="s">
         <v>176</v>
@@ -7500,10 +7503,10 @@
         <v>128</v>
       </c>
       <c r="B233" s="6" t="s">
-        <v>847</v>
+        <v>762</v>
       </c>
       <c r="C233" s="6" t="s">
-        <v>849</v>
+        <v>764</v>
       </c>
       <c r="D233" s="17" t="s">
         <v>176</v>
@@ -7514,10 +7517,10 @@
         <v>128</v>
       </c>
       <c r="B234" s="6" t="s">
-        <v>851</v>
+        <v>766</v>
       </c>
       <c r="C234" s="6" t="s">
-        <v>848</v>
+        <v>763</v>
       </c>
       <c r="D234" s="11" t="s">
         <v>409</v>
@@ -7528,10 +7531,10 @@
         <v>128</v>
       </c>
       <c r="B235" s="6" t="s">
-        <v>852</v>
+        <v>767</v>
       </c>
       <c r="C235" s="6" t="s">
-        <v>856</v>
+        <v>771</v>
       </c>
       <c r="D235" s="11" t="s">
         <v>411</v>
@@ -7542,10 +7545,10 @@
         <v>128</v>
       </c>
       <c r="B236" s="6" t="s">
-        <v>853</v>
+        <v>768</v>
       </c>
       <c r="C236" s="6" t="s">
-        <v>857</v>
+        <v>772</v>
       </c>
       <c r="D236" s="11" t="s">
         <v>385</v>
@@ -7556,10 +7559,10 @@
         <v>128</v>
       </c>
       <c r="B237" s="6" t="s">
-        <v>854</v>
+        <v>769</v>
       </c>
       <c r="C237" s="6" t="s">
-        <v>858</v>
+        <v>773</v>
       </c>
       <c r="D237" s="11" t="s">
         <v>398</v>
@@ -7570,10 +7573,10 @@
         <v>128</v>
       </c>
       <c r="B238" s="6" t="s">
-        <v>855</v>
+        <v>770</v>
       </c>
       <c r="C238" s="6" t="s">
-        <v>859</v>
+        <v>774</v>
       </c>
       <c r="D238" s="11" t="s">
         <v>405</v>
@@ -7584,10 +7587,10 @@
         <v>128</v>
       </c>
       <c r="B239" s="6" t="s">
-        <v>841</v>
+        <v>756</v>
       </c>
       <c r="C239" s="6" t="s">
-        <v>887</v>
+        <v>802</v>
       </c>
       <c r="D239" s="11" t="s">
         <v>176</v>
@@ -7601,10 +7604,10 @@
         <v>128</v>
       </c>
       <c r="B240" s="6" t="s">
-        <v>840</v>
+        <v>755</v>
       </c>
       <c r="C240" s="6" t="s">
-        <v>888</v>
+        <v>803</v>
       </c>
       <c r="D240" s="17" t="s">
         <v>176</v>
@@ -7615,10 +7618,10 @@
         <v>128</v>
       </c>
       <c r="B241" s="6" t="s">
-        <v>831</v>
+        <v>746</v>
       </c>
       <c r="C241" s="6" t="s">
-        <v>889</v>
+        <v>804</v>
       </c>
       <c r="D241" s="11" t="s">
         <v>381</v>
@@ -7629,10 +7632,10 @@
         <v>128</v>
       </c>
       <c r="B242" s="6" t="s">
-        <v>832</v>
+        <v>747</v>
       </c>
       <c r="C242" s="6" t="s">
-        <v>890</v>
+        <v>805</v>
       </c>
       <c r="D242" s="11" t="s">
         <v>383</v>
@@ -7643,10 +7646,10 @@
         <v>128</v>
       </c>
       <c r="B243" s="6" t="s">
-        <v>833</v>
+        <v>748</v>
       </c>
       <c r="C243" s="6" t="s">
-        <v>891</v>
+        <v>806</v>
       </c>
       <c r="D243" s="11" t="s">
         <v>385</v>
@@ -7657,10 +7660,10 @@
         <v>128</v>
       </c>
       <c r="B244" s="6" t="s">
-        <v>828</v>
+        <v>743</v>
       </c>
       <c r="C244" s="6" t="s">
-        <v>892</v>
+        <v>807</v>
       </c>
       <c r="D244" s="11" t="s">
         <v>413</v>
@@ -7671,10 +7674,10 @@
         <v>128</v>
       </c>
       <c r="B245" s="6" t="s">
-        <v>829</v>
+        <v>744</v>
       </c>
       <c r="C245" s="6" t="s">
-        <v>893</v>
+        <v>808</v>
       </c>
       <c r="D245" s="11" t="s">
         <v>415</v>
@@ -7685,10 +7688,10 @@
         <v>128</v>
       </c>
       <c r="B246" s="6" t="s">
-        <v>830</v>
+        <v>745</v>
       </c>
       <c r="C246" s="6" t="s">
-        <v>894</v>
+        <v>809</v>
       </c>
       <c r="D246" s="11" t="s">
         <v>417</v>
@@ -7699,10 +7702,10 @@
         <v>128</v>
       </c>
       <c r="B247" s="6" t="s">
-        <v>836</v>
+        <v>751</v>
       </c>
       <c r="C247" s="6" t="s">
-        <v>895</v>
+        <v>810</v>
       </c>
       <c r="D247" s="11" t="s">
         <v>390</v>
@@ -7713,10 +7716,10 @@
         <v>128</v>
       </c>
       <c r="B248" s="6" t="s">
-        <v>837</v>
+        <v>752</v>
       </c>
       <c r="C248" s="6" t="s">
-        <v>896</v>
+        <v>811</v>
       </c>
       <c r="D248" s="11" t="s">
         <v>392</v>
@@ -7727,10 +7730,10 @@
         <v>128</v>
       </c>
       <c r="B249" s="6" t="s">
-        <v>838</v>
+        <v>753</v>
       </c>
       <c r="C249" s="6" t="s">
-        <v>897</v>
+        <v>812</v>
       </c>
       <c r="D249" s="11" t="s">
         <v>394</v>
@@ -7741,10 +7744,10 @@
         <v>128</v>
       </c>
       <c r="B250" s="6" t="s">
-        <v>835</v>
+        <v>750</v>
       </c>
       <c r="C250" s="6" t="s">
-        <v>898</v>
+        <v>813</v>
       </c>
       <c r="D250" s="11" t="s">
         <v>396</v>
@@ -7755,10 +7758,10 @@
         <v>128</v>
       </c>
       <c r="B251" s="6" t="s">
-        <v>839</v>
+        <v>754</v>
       </c>
       <c r="C251" s="6" t="s">
-        <v>899</v>
+        <v>814</v>
       </c>
       <c r="D251" s="11" t="s">
         <v>398</v>
@@ -7769,10 +7772,10 @@
         <v>128</v>
       </c>
       <c r="B252" s="6" t="s">
-        <v>845</v>
+        <v>760</v>
       </c>
       <c r="C252" s="6" t="s">
-        <v>900</v>
+        <v>815</v>
       </c>
       <c r="D252" s="11" t="s">
         <v>405</v>
@@ -7783,10 +7786,10 @@
         <v>128</v>
       </c>
       <c r="B253" s="6" t="s">
-        <v>826</v>
+        <v>741</v>
       </c>
       <c r="C253" s="6" t="s">
-        <v>825</v>
+        <v>740</v>
       </c>
       <c r="D253" s="11" t="s">
         <v>417</v>
@@ -7797,10 +7800,10 @@
         <v>128</v>
       </c>
       <c r="B254" s="6" t="s">
-        <v>824</v>
+        <v>739</v>
       </c>
       <c r="C254" s="6" t="s">
-        <v>825</v>
+        <v>740</v>
       </c>
       <c r="D254" s="11" t="s">
         <v>439</v>
@@ -9074,7 +9077,7 @@
         <v>220</v>
       </c>
       <c r="E17" t="s">
-        <v>698</v>
+        <v>688</v>
       </c>
       <c r="F17" t="s">
         <v>420</v>
@@ -10551,10 +10554,10 @@
         <v>484</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>821</v>
+        <v>736</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>804</v>
+        <v>719</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>420</v>
@@ -10800,10 +10803,10 @@
         <v>470</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>809</v>
+        <v>724</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>810</v>
+        <v>725</v>
       </c>
       <c r="F2" t="s">
         <v>420</v>
@@ -10820,10 +10823,10 @@
         <v>471</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>806</v>
+        <v>721</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>810</v>
+        <v>725</v>
       </c>
       <c r="F3" t="s">
         <v>420</v>
@@ -10840,10 +10843,10 @@
         <v>472</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>805</v>
+        <v>720</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>804</v>
+        <v>719</v>
       </c>
       <c r="F4" t="s">
         <v>420</v>
@@ -10963,7 +10966,7 @@
         <v>448</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>844</v>
+        <v>759</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>420</v>
@@ -11262,7 +11265,7 @@
         <v>464</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>834</v>
+        <v>749</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>427</v>

</xml_diff>

<commit_message>
Replaced double quotes with single quotes
</commit_message>
<xml_diff>
--- a/docs/coverage-testing/85b_test_definitions_PIV_ICAM_Test_Cards_Exploded.xlsx
+++ b/docs/coverage-testing/85b_test_definitions_PIV_ICAM_Test_Cards_Exploded.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\docs\coverage-testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10450041-0639-46A5-A9DB-E05909B8D01E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860881D9-1E13-4316-871E-5F30C1DC6AB6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2775" yWindow="255" windowWidth="23700" windowHeight="15240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2341,9 +2341,6 @@
     <t>sp800_76Test_39</t>
   </si>
   <si>
-    <t>Verify that that the CBEFF Creation Date is encoded in 8 bytes using a binary representation of "YYYYMMDDhhmmssZ"</t>
-  </si>
-  <si>
     <t>sp800_76Test_40</t>
   </si>
   <si>
@@ -2399,9 +2396,6 @@
   </si>
   <si>
     <t>sp800_76Test_47</t>
-  </si>
-  <si>
-    <t>Verify that that the facial image CBEFF Creation Date is encoded in 8 bytes using a binary representation of "YYYYMMDDhhmmssZ"</t>
   </si>
   <si>
     <t>76.48</t>
@@ -3014,6 +3008,12 @@
   </si>
   <si>
     <t>8.10.1.4</t>
+  </si>
+  <si>
+    <t>Verify that that the CBEFF Creation Date is encoded in 8 bytes using a binary representation of 'YYYYMMDDhhmmssZ'</t>
+  </si>
+  <si>
+    <t>Verify that that the facial image CBEFF Creation Date is encoded in 8 bytes using a binary representation of 'YYYYMMDDhhmmssZ'</t>
   </si>
 </sst>
 </file>
@@ -5405,7 +5405,7 @@
   <dimension ref="A1:F287"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D27" sqref="D1:D1048576"/>
+      <selection activeCell="C27" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5441,7 +5441,7 @@
         <v>129</v>
       </c>
       <c r="B2" s="58" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="C2" s="58" t="s">
         <v>131</v>
@@ -5459,7 +5459,7 @@
         <v>129</v>
       </c>
       <c r="B3" s="58" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="C3" s="58" t="s">
         <v>135</v>
@@ -5475,7 +5475,7 @@
         <v>129</v>
       </c>
       <c r="B4" s="58" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="C4" s="58" t="s">
         <v>138</v>
@@ -5491,7 +5491,7 @@
         <v>129</v>
       </c>
       <c r="B5" s="58" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="C5" s="58" t="s">
         <v>140</v>
@@ -5619,7 +5619,7 @@
         <v>129</v>
       </c>
       <c r="B13" s="68" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="C13" s="58" t="s">
         <v>161</v>
@@ -5635,7 +5635,7 @@
         <v>129</v>
       </c>
       <c r="B14" s="68" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="C14" s="58" t="s">
         <v>135</v>
@@ -5651,7 +5651,7 @@
         <v>129</v>
       </c>
       <c r="B15" s="68" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="C15" s="58" t="s">
         <v>138</v>
@@ -5667,7 +5667,7 @@
         <v>129</v>
       </c>
       <c r="B16" s="68" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="C16" s="58" t="s">
         <v>140</v>
@@ -5699,7 +5699,7 @@
         <v>129</v>
       </c>
       <c r="B18" s="68" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="C18" s="68" t="s">
         <v>170</v>
@@ -5715,7 +5715,7 @@
         <v>129</v>
       </c>
       <c r="B19" s="68" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="C19" s="68" t="s">
         <v>172</v>
@@ -5731,7 +5731,7 @@
         <v>129</v>
       </c>
       <c r="B20" s="68" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="C20" s="58" t="s">
         <v>174</v>
@@ -5747,7 +5747,7 @@
         <v>129</v>
       </c>
       <c r="B21" s="68" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="C21" s="58" t="s">
         <v>176</v>
@@ -5763,7 +5763,7 @@
         <v>129</v>
       </c>
       <c r="B22" s="68" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="C22" s="58" t="s">
         <v>178</v>
@@ -5779,7 +5779,7 @@
         <v>129</v>
       </c>
       <c r="B23" s="68" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="C23" s="58" t="s">
         <v>168</v>
@@ -5830,7 +5830,7 @@
         <v>164</v>
       </c>
       <c r="C26" s="68" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="D26" s="69" t="s">
         <v>177</v>
@@ -5859,7 +5859,7 @@
         <v>129</v>
       </c>
       <c r="B28" s="58" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="C28" s="58" t="s">
         <v>184</v>
@@ -5875,7 +5875,7 @@
         <v>129</v>
       </c>
       <c r="B29" s="68" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="C29" s="58" t="s">
         <v>187</v>
@@ -5891,7 +5891,7 @@
         <v>129</v>
       </c>
       <c r="B30" s="68" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="C30" s="58" t="s">
         <v>135</v>
@@ -5907,7 +5907,7 @@
         <v>129</v>
       </c>
       <c r="B31" s="68" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C31" s="58" t="s">
         <v>138</v>
@@ -5923,7 +5923,7 @@
         <v>129</v>
       </c>
       <c r="B32" s="68" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="C32" s="58" t="s">
         <v>140</v>
@@ -5955,7 +5955,7 @@
         <v>129</v>
       </c>
       <c r="B34" s="68" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="C34" s="58" t="s">
         <v>190</v>
@@ -5971,7 +5971,7 @@
         <v>129</v>
       </c>
       <c r="B35" s="68" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="C35" s="58" t="s">
         <v>192</v>
@@ -5987,7 +5987,7 @@
         <v>129</v>
       </c>
       <c r="B36" s="68" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="C36" s="58" t="s">
         <v>194</v>
@@ -6003,7 +6003,7 @@
         <v>129</v>
       </c>
       <c r="B37" s="68" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="C37" s="58" t="s">
         <v>196</v>
@@ -6019,7 +6019,7 @@
         <v>129</v>
       </c>
       <c r="B38" s="68" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="C38" s="58" t="s">
         <v>184</v>
@@ -6035,7 +6035,7 @@
         <v>129</v>
       </c>
       <c r="B39" s="68" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="C39" s="58" t="s">
         <v>198</v>
@@ -6051,7 +6051,7 @@
         <v>129</v>
       </c>
       <c r="B40" s="68" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="C40" s="58" t="s">
         <v>135</v>
@@ -6067,7 +6067,7 @@
         <v>129</v>
       </c>
       <c r="B41" s="68" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="C41" s="58" t="s">
         <v>138</v>
@@ -6083,7 +6083,7 @@
         <v>129</v>
       </c>
       <c r="B42" s="68" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="C42" s="58" t="s">
         <v>140</v>
@@ -6179,7 +6179,7 @@
         <v>129</v>
       </c>
       <c r="B48" s="68" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="C48" s="58" t="s">
         <v>208</v>
@@ -6195,7 +6195,7 @@
         <v>129</v>
       </c>
       <c r="B49" s="68" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="C49" s="58" t="s">
         <v>135</v>
@@ -6211,7 +6211,7 @@
         <v>129</v>
       </c>
       <c r="B50" s="68" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="C50" s="58" t="s">
         <v>138</v>
@@ -6227,7 +6227,7 @@
         <v>129</v>
       </c>
       <c r="B51" s="68" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="C51" s="58" t="s">
         <v>140</v>
@@ -6243,7 +6243,7 @@
         <v>129</v>
       </c>
       <c r="B52" s="68" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="C52" s="58" t="s">
         <v>209</v>
@@ -6259,7 +6259,7 @@
         <v>129</v>
       </c>
       <c r="B53" s="68" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="C53" s="58" t="s">
         <v>211</v>
@@ -6275,7 +6275,7 @@
         <v>129</v>
       </c>
       <c r="B54" s="68" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="C54" s="58" t="s">
         <v>213</v>
@@ -6291,7 +6291,7 @@
         <v>129</v>
       </c>
       <c r="B55" s="68" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="C55" s="58" t="s">
         <v>215</v>
@@ -6307,7 +6307,7 @@
         <v>129</v>
       </c>
       <c r="B56" s="68" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="C56" s="58" t="s">
         <v>217</v>
@@ -6323,7 +6323,7 @@
         <v>129</v>
       </c>
       <c r="B57" s="68" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="C57" s="58" t="s">
         <v>184</v>
@@ -6339,7 +6339,7 @@
         <v>129</v>
       </c>
       <c r="B58" s="68" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="C58" s="58" t="s">
         <v>219</v>
@@ -6355,7 +6355,7 @@
         <v>129</v>
       </c>
       <c r="B59" s="68" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="C59" s="58" t="s">
         <v>135</v>
@@ -6371,7 +6371,7 @@
         <v>129</v>
       </c>
       <c r="B60" s="68" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="C60" s="58" t="s">
         <v>138</v>
@@ -6387,7 +6387,7 @@
         <v>129</v>
       </c>
       <c r="B61" s="68" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="C61" s="58" t="s">
         <v>140</v>
@@ -6403,7 +6403,7 @@
         <v>129</v>
       </c>
       <c r="B62" s="68" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="C62" s="58" t="s">
         <v>220</v>
@@ -6419,7 +6419,7 @@
         <v>129</v>
       </c>
       <c r="B63" s="68" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="C63" s="58" t="s">
         <v>222</v>
@@ -6435,7 +6435,7 @@
         <v>129</v>
       </c>
       <c r="B64" s="68" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="C64" s="58" t="s">
         <v>224</v>
@@ -6451,7 +6451,7 @@
         <v>129</v>
       </c>
       <c r="B65" s="68" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="C65" s="58" t="s">
         <v>184</v>
@@ -6467,7 +6467,7 @@
         <v>129</v>
       </c>
       <c r="B66" s="68" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="C66" s="58" t="s">
         <v>226</v>
@@ -6485,7 +6485,7 @@
         <v>129</v>
       </c>
       <c r="B67" s="68" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="C67" s="58" t="s">
         <v>135</v>
@@ -6501,7 +6501,7 @@
         <v>129</v>
       </c>
       <c r="B68" s="68" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="C68" s="58" t="s">
         <v>138</v>
@@ -6517,7 +6517,7 @@
         <v>129</v>
       </c>
       <c r="B69" s="68" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="C69" s="58" t="s">
         <v>140</v>
@@ -6533,7 +6533,7 @@
         <v>129</v>
       </c>
       <c r="B70" s="68" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="C70" s="58" t="s">
         <v>188</v>
@@ -6549,7 +6549,7 @@
         <v>129</v>
       </c>
       <c r="B71" s="68" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="C71" s="58" t="s">
         <v>190</v>
@@ -6565,7 +6565,7 @@
         <v>129</v>
       </c>
       <c r="B72" s="68" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="C72" s="58" t="s">
         <v>192</v>
@@ -6581,7 +6581,7 @@
         <v>129</v>
       </c>
       <c r="B73" s="68" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="C73" s="58" t="s">
         <v>196</v>
@@ -6597,7 +6597,7 @@
         <v>129</v>
       </c>
       <c r="B74" s="68" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="C74" s="58" t="s">
         <v>194</v>
@@ -6613,7 +6613,7 @@
         <v>129</v>
       </c>
       <c r="B75" s="68" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="C75" s="58" t="s">
         <v>184</v>
@@ -6629,7 +6629,7 @@
         <v>129</v>
       </c>
       <c r="B76" s="68" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="C76" s="58" t="s">
         <v>227</v>
@@ -6647,7 +6647,7 @@
         <v>129</v>
       </c>
       <c r="B77" s="68" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="C77" s="58" t="s">
         <v>135</v>
@@ -6663,7 +6663,7 @@
         <v>129</v>
       </c>
       <c r="B78" s="68" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="C78" s="58" t="s">
         <v>138</v>
@@ -6679,7 +6679,7 @@
         <v>129</v>
       </c>
       <c r="B79" s="68" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="C79" s="58" t="s">
         <v>140</v>
@@ -6695,7 +6695,7 @@
         <v>129</v>
       </c>
       <c r="B80" s="68" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="C80" s="58" t="s">
         <v>188</v>
@@ -6711,7 +6711,7 @@
         <v>129</v>
       </c>
       <c r="B81" s="68" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="C81" s="58" t="s">
         <v>190</v>
@@ -6727,7 +6727,7 @@
         <v>129</v>
       </c>
       <c r="B82" s="68" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="C82" s="58" t="s">
         <v>192</v>
@@ -6743,7 +6743,7 @@
         <v>129</v>
       </c>
       <c r="B83" s="68" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="C83" s="58" t="s">
         <v>194</v>
@@ -6759,7 +6759,7 @@
         <v>129</v>
       </c>
       <c r="B84" s="68" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="C84" s="58" t="s">
         <v>196</v>
@@ -6775,7 +6775,7 @@
         <v>129</v>
       </c>
       <c r="B85" s="68" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="C85" s="58" t="s">
         <v>184</v>
@@ -6791,7 +6791,7 @@
         <v>129</v>
       </c>
       <c r="B86" s="68" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="C86" s="58" t="s">
         <v>228</v>
@@ -6809,7 +6809,7 @@
         <v>129</v>
       </c>
       <c r="B87" s="68" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="C87" s="58" t="s">
         <v>135</v>
@@ -6825,7 +6825,7 @@
         <v>129</v>
       </c>
       <c r="B88" s="68" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="C88" s="58" t="s">
         <v>138</v>
@@ -6841,7 +6841,7 @@
         <v>129</v>
       </c>
       <c r="B89" s="68" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="C89" s="58" t="s">
         <v>140</v>
@@ -6857,7 +6857,7 @@
         <v>129</v>
       </c>
       <c r="B90" s="68" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="C90" s="58" t="s">
         <v>188</v>
@@ -6873,7 +6873,7 @@
         <v>129</v>
       </c>
       <c r="B91" s="68" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="C91" s="58" t="s">
         <v>190</v>
@@ -6889,7 +6889,7 @@
         <v>129</v>
       </c>
       <c r="B92" s="68" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="C92" s="58" t="s">
         <v>192</v>
@@ -6905,7 +6905,7 @@
         <v>129</v>
       </c>
       <c r="B93" s="68" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="C93" s="58" t="s">
         <v>194</v>
@@ -6921,7 +6921,7 @@
         <v>129</v>
       </c>
       <c r="B94" s="68" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="C94" s="58" t="s">
         <v>196</v>
@@ -6937,7 +6937,7 @@
         <v>129</v>
       </c>
       <c r="B95" s="68" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="C95" s="58" t="s">
         <v>184</v>
@@ -6953,7 +6953,7 @@
         <v>129</v>
       </c>
       <c r="B96" s="68" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="C96" s="58" t="s">
         <v>229</v>
@@ -6971,7 +6971,7 @@
         <v>129</v>
       </c>
       <c r="B97" s="68" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="C97" s="58" t="s">
         <v>135</v>
@@ -6987,7 +6987,7 @@
         <v>129</v>
       </c>
       <c r="B98" s="68" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="C98" s="58" t="s">
         <v>138</v>
@@ -7003,7 +7003,7 @@
         <v>129</v>
       </c>
       <c r="B99" s="68" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="C99" s="58" t="s">
         <v>140</v>
@@ -7019,7 +7019,7 @@
         <v>129</v>
       </c>
       <c r="B100" s="68" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="C100" s="58" t="s">
         <v>230</v>
@@ -7035,7 +7035,7 @@
         <v>129</v>
       </c>
       <c r="B101" s="68" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="C101" s="58" t="s">
         <v>232</v>
@@ -7051,7 +7051,7 @@
         <v>129</v>
       </c>
       <c r="B102" s="68" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="C102" s="58" t="s">
         <v>234</v>
@@ -7067,7 +7067,7 @@
         <v>129</v>
       </c>
       <c r="B103" s="68" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="C103" s="58" t="s">
         <v>236</v>
@@ -11805,7 +11805,7 @@
         <v>763</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>764</v>
+        <v>982</v>
       </c>
       <c r="E40" s="18"/>
       <c r="F40" s="3"/>
@@ -11819,10 +11819,10 @@
         <v>695</v>
       </c>
       <c r="C41" s="17" t="s">
+        <v>764</v>
+      </c>
+      <c r="D41" s="14" t="s">
         <v>765</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>766</v>
       </c>
       <c r="E41" s="18"/>
       <c r="F41" s="3"/>
@@ -11836,13 +11836,13 @@
         <v>695</v>
       </c>
       <c r="C42" s="17" t="s">
+        <v>766</v>
+      </c>
+      <c r="D42" s="14" t="s">
         <v>767</v>
       </c>
-      <c r="D42" s="14" t="s">
+      <c r="E42" s="14" t="s">
         <v>768</v>
-      </c>
-      <c r="E42" s="14" t="s">
-        <v>769</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
@@ -11855,13 +11855,13 @@
         <v>695</v>
       </c>
       <c r="C43" s="17" t="s">
+        <v>769</v>
+      </c>
+      <c r="D43" s="14" t="s">
         <v>770</v>
       </c>
-      <c r="D43" s="14" t="s">
+      <c r="E43" s="14" t="s">
         <v>771</v>
-      </c>
-      <c r="E43" s="14" t="s">
-        <v>772</v>
       </c>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
@@ -11874,13 +11874,13 @@
         <v>695</v>
       </c>
       <c r="C44" s="17" t="s">
+        <v>772</v>
+      </c>
+      <c r="D44" s="14" t="s">
         <v>773</v>
       </c>
-      <c r="D44" s="14" t="s">
+      <c r="E44" s="14" t="s">
         <v>774</v>
-      </c>
-      <c r="E44" s="14" t="s">
-        <v>775</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
@@ -11893,10 +11893,10 @@
         <v>695</v>
       </c>
       <c r="C45" s="17" t="s">
+        <v>775</v>
+      </c>
+      <c r="D45" s="14" t="s">
         <v>776</v>
-      </c>
-      <c r="D45" s="14" t="s">
-        <v>777</v>
       </c>
       <c r="E45" s="18"/>
       <c r="F45" s="3"/>
@@ -11910,10 +11910,10 @@
         <v>695</v>
       </c>
       <c r="C46" s="17" t="s">
+        <v>777</v>
+      </c>
+      <c r="D46" s="14" t="s">
         <v>778</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>779</v>
       </c>
       <c r="E46" s="18"/>
       <c r="F46" s="3"/>
@@ -11927,10 +11927,10 @@
         <v>695</v>
       </c>
       <c r="C47" s="17" t="s">
+        <v>779</v>
+      </c>
+      <c r="D47" s="14" t="s">
         <v>780</v>
-      </c>
-      <c r="D47" s="14" t="s">
-        <v>781</v>
       </c>
       <c r="E47" s="18"/>
       <c r="F47" s="3"/>
@@ -11938,16 +11938,16 @@
     </row>
     <row r="48" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B48" s="17" t="s">
         <v>695</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>784</v>
+        <v>983</v>
       </c>
       <c r="E48" s="18"/>
       <c r="F48" s="3"/>
@@ -11955,16 +11955,16 @@
     </row>
     <row r="49" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="B49" s="17" t="s">
         <v>695</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="E49" s="18"/>
       <c r="F49" s="3"/>
@@ -11972,16 +11972,16 @@
     </row>
     <row r="50" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="B50" s="17" t="s">
         <v>695</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="E50" s="18"/>
       <c r="F50" s="3"/>
@@ -11989,19 +11989,19 @@
     </row>
     <row r="51" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="B51" s="17" t="s">
         <v>695</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="E51" s="14" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
@@ -12063,13 +12063,13 @@
         <v>390</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>792</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>793</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>794</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>795</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>796</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="14" t="s">
@@ -12082,13 +12082,13 @@
         <v>393</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="14" t="s">
@@ -12101,13 +12101,13 @@
         <v>396</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="14" t="s">
@@ -12120,13 +12120,13 @@
         <v>411</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="14" t="s">
@@ -12139,13 +12139,13 @@
         <v>399</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="14" t="s">
@@ -12158,13 +12158,13 @@
         <v>402</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="14" t="s">
@@ -12177,13 +12177,13 @@
         <v>405</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="14" t="s">
@@ -12196,13 +12196,13 @@
         <v>408</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="14" t="s">
@@ -12215,13 +12215,13 @@
         <v>414</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="14" t="s">
@@ -12231,16 +12231,16 @@
     </row>
     <row r="11" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
+        <v>811</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>792</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>812</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>813</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>794</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>814</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>815</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="14" t="s">
@@ -12253,13 +12253,13 @@
         <v>417</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="E12" s="32"/>
       <c r="F12" s="14" t="s">
@@ -12272,22 +12272,22 @@
         <v>420</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C13" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>817</v>
+      </c>
+      <c r="E13" s="34" t="s">
         <v>818</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="F13" s="35" t="s">
+        <v>241</v>
+      </c>
+      <c r="G13" s="14" t="s">
         <v>819</v>
-      </c>
-      <c r="E13" s="34" t="s">
-        <v>820</v>
-      </c>
-      <c r="F13" s="35" t="s">
-        <v>241</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>821</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -12295,13 +12295,13 @@
         <v>423</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="E14" s="36"/>
       <c r="F14" s="14" t="s">
@@ -12314,22 +12314,22 @@
         <v>426</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>459</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="F15" s="14" t="s">
         <v>241</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12337,13 +12337,13 @@
         <v>453</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="E16" s="14"/>
       <c r="F16" s="14" t="s">
@@ -12356,22 +12356,22 @@
         <v>462</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>461</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="F17" s="14" t="s">
         <v>241</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -12379,10 +12379,10 @@
         <v>493</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>492</v>
@@ -12398,10 +12398,10 @@
         <v>496</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>495</v>
@@ -12417,13 +12417,13 @@
         <v>499</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="14" t="s">
@@ -12436,13 +12436,13 @@
         <v>502</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="14" t="s">
@@ -12455,13 +12455,13 @@
         <v>507</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="E22" s="15"/>
       <c r="F22" s="14" t="s">
@@ -12474,10 +12474,10 @@
         <v>447</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>504</v>
@@ -12539,16 +12539,16 @@
         <v>429</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>839</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>840</v>
+      </c>
+      <c r="D2" s="39" t="s">
         <v>841</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="E2" s="40" t="s">
         <v>842</v>
-      </c>
-      <c r="D2" s="39" t="s">
-        <v>843</v>
-      </c>
-      <c r="E2" s="40" t="s">
-        <v>844</v>
       </c>
       <c r="F2" s="41" t="s">
         <v>241</v>
@@ -12560,16 +12560,16 @@
         <v>467</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="F3" s="41" t="s">
         <v>241</v>
@@ -12581,16 +12581,16 @@
         <v>450</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="E4" s="42" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="F4" s="41" t="s">
         <v>241</v>
@@ -12705,20 +12705,20 @@
         <v>510</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>847</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>848</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>849</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>850</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>851</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="14" t="s">
         <v>241</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -12726,13 +12726,13 @@
         <v>562</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="14" t="s">
@@ -12745,10 +12745,10 @@
         <v>519</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>518</v>
@@ -12764,10 +12764,10 @@
         <v>522</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>521</v>
@@ -12783,10 +12783,10 @@
         <v>525</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>524</v>
@@ -12802,22 +12802,22 @@
         <v>528</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="D7" s="48" t="s">
         <v>527</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="F7" s="35" t="s">
         <v>241</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -12825,13 +12825,13 @@
         <v>531</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="E8" s="49"/>
       <c r="F8" s="14" t="s">
@@ -12844,13 +12844,13 @@
         <v>534</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="E9" s="46"/>
       <c r="F9" s="14" t="s">
@@ -12863,13 +12863,13 @@
         <v>537</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="E10" s="46"/>
       <c r="F10" s="14" t="s">
@@ -12882,10 +12882,10 @@
         <v>540</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>539</v>
@@ -12901,10 +12901,10 @@
         <v>543</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>542</v>
@@ -12914,7 +12914,7 @@
         <v>241</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -12922,22 +12922,22 @@
         <v>546</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C13" s="14" t="s">
+        <v>868</v>
+      </c>
+      <c r="D13" s="48" t="s">
+        <v>869</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>828</v>
+      </c>
+      <c r="F13" s="35" t="s">
+        <v>241</v>
+      </c>
+      <c r="G13" s="14" t="s">
         <v>870</v>
-      </c>
-      <c r="D13" s="48" t="s">
-        <v>871</v>
-      </c>
-      <c r="E13" s="34" t="s">
-        <v>830</v>
-      </c>
-      <c r="F13" s="35" t="s">
-        <v>241</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>872</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -12945,22 +12945,22 @@
         <v>553</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="D14" s="48" t="s">
         <v>552</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="F14" s="35" t="s">
         <v>241</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -12968,10 +12968,10 @@
         <v>556</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>555</v>
@@ -12987,13 +12987,13 @@
         <v>565</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="E16" s="46"/>
       <c r="F16" s="14" t="s">
@@ -13006,13 +13006,13 @@
         <v>582</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="E17" s="46"/>
       <c r="F17" s="14" t="s">
@@ -13025,13 +13025,13 @@
         <v>568</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="E18" s="47"/>
       <c r="F18" s="14" t="s">
@@ -13044,22 +13044,22 @@
         <v>603</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C19" s="14" t="s">
+        <v>881</v>
+      </c>
+      <c r="D19" s="48" t="s">
+        <v>882</v>
+      </c>
+      <c r="E19" s="34" t="s">
         <v>883</v>
       </c>
-      <c r="D19" s="48" t="s">
+      <c r="F19" s="35" t="s">
+        <v>241</v>
+      </c>
+      <c r="G19" s="14" t="s">
         <v>884</v>
-      </c>
-      <c r="E19" s="34" t="s">
-        <v>885</v>
-      </c>
-      <c r="F19" s="35" t="s">
-        <v>241</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>886</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -13067,13 +13067,13 @@
         <v>606</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="E20" s="50"/>
       <c r="F20" s="14" t="s">
@@ -13086,22 +13086,22 @@
         <v>609</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C21" s="38" t="s">
+        <v>887</v>
+      </c>
+      <c r="D21" s="51" t="s">
+        <v>888</v>
+      </c>
+      <c r="E21" s="34" t="s">
         <v>889</v>
       </c>
-      <c r="D21" s="51" t="s">
+      <c r="F21" s="52" t="s">
+        <v>241</v>
+      </c>
+      <c r="G21" s="38" t="s">
         <v>890</v>
-      </c>
-      <c r="E21" s="34" t="s">
-        <v>891</v>
-      </c>
-      <c r="F21" s="52" t="s">
-        <v>241</v>
-      </c>
-      <c r="G21" s="38" t="s">
-        <v>892</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -13109,22 +13109,22 @@
         <v>624</v>
       </c>
       <c r="B22" s="54" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C22" s="55" t="s">
+        <v>891</v>
+      </c>
+      <c r="D22" s="55" t="s">
+        <v>892</v>
+      </c>
+      <c r="E22" s="55" t="s">
         <v>893</v>
-      </c>
-      <c r="D22" s="55" t="s">
-        <v>894</v>
-      </c>
-      <c r="E22" s="55" t="s">
-        <v>895</v>
       </c>
       <c r="F22" s="55" t="s">
         <v>133</v>
       </c>
       <c r="G22" s="56" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
     </row>
   </sheetData>
@@ -13152,7 +13152,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>126</v>
@@ -14136,7 +14136,7 @@
     </row>
     <row r="101" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="14" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="B101" s="15"/>
       <c r="C101" s="15"/>
@@ -14145,7 +14145,7 @@
     </row>
     <row r="102" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="14" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="B102" s="15"/>
       <c r="C102" s="15"/>

</xml_diff>

<commit_message>
Replaced all double quotes with triple double quotes
</commit_message>
<xml_diff>
--- a/docs/coverage-testing/85b_test_definitions_PIV_ICAM_Test_Cards_Exploded.xlsx
+++ b/docs/coverage-testing/85b_test_definitions_PIV_ICAM_Test_Cards_Exploded.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\docs\coverage-testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73827C96-9791-45D6-AC8E-B0DAC7594516}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCDE82E-A41F-426B-839E-79B4856C2E63}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2775" yWindow="255" windowWidth="23700" windowHeight="15240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2775" yWindow="255" windowWidth="23700" windowHeight="15240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIV I Reference Tests" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2254" uniqueCount="984">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2253" uniqueCount="985">
   <si>
     <t>Test Case</t>
   </si>
@@ -2329,9 +2329,6 @@
     <t>sp800_76Test_39</t>
   </si>
   <si>
-    <t>Verify that that the CBEFF Creation Date is encoded in 8 bytes using a binary representation of "YYYYMMDDhhmmssZ"</t>
-  </si>
-  <si>
     <t>sp800_76Test_40</t>
   </si>
   <si>
@@ -2387,9 +2384,6 @@
   </si>
   <si>
     <t>sp800_76Test_47</t>
-  </si>
-  <si>
-    <t>Verify that that the facial image CBEFF Creation Date is encoded in 8 bytes using a binary representation of "YYYYMMDDhhmmssZ"</t>
   </si>
   <si>
     <t>76.48</t>
@@ -3014,6 +3008,15 @@
   </si>
   <si>
     <t>Test is there but I am not 100% sure if that is enough, might require additional checks</t>
+  </si>
+  <si>
+    <t>CCC Tag 0xFE present and after any tags from 73-4.4 and 73-4.5</t>
+  </si>
+  <si>
+    <t>Verify that that the CBEFF Creation Date is encoded in 8 bytes using a binary representation of """YYYYMMDDhhmmssZ"""</t>
+  </si>
+  <si>
+    <t>Verify that that the facial image CBEFF Creation Date is encoded in 8 bytes using a binary representation of """YYYYMMDDhhmmssZ"""</t>
   </si>
 </sst>
 </file>
@@ -3293,7 +3296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -3456,6 +3459,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5453,7 +5459,7 @@
         <v>129</v>
       </c>
       <c r="B2" s="52" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="C2" s="52" t="s">
         <v>131</v>
@@ -5471,7 +5477,7 @@
         <v>129</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="C3" s="52" t="s">
         <v>135</v>
@@ -5487,7 +5493,7 @@
         <v>129</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="C4" s="52" t="s">
         <v>138</v>
@@ -5503,7 +5509,7 @@
         <v>129</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="C5" s="52" t="s">
         <v>140</v>
@@ -5538,7 +5544,7 @@
         <v>134</v>
       </c>
       <c r="C7" s="52" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="D7" s="52" t="s">
         <v>144</v>
@@ -5631,7 +5637,7 @@
         <v>129</v>
       </c>
       <c r="B13" s="62" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="C13" s="52" t="s">
         <v>160</v>
@@ -5647,7 +5653,7 @@
         <v>129</v>
       </c>
       <c r="B14" s="62" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="C14" s="52" t="s">
         <v>135</v>
@@ -5663,7 +5669,7 @@
         <v>129</v>
       </c>
       <c r="B15" s="62" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="C15" s="52" t="s">
         <v>138</v>
@@ -5679,7 +5685,7 @@
         <v>129</v>
       </c>
       <c r="B16" s="62" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="C16" s="52" t="s">
         <v>140</v>
@@ -5711,7 +5717,7 @@
         <v>129</v>
       </c>
       <c r="B18" s="62" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="C18" s="62" t="s">
         <v>169</v>
@@ -5727,7 +5733,7 @@
         <v>129</v>
       </c>
       <c r="B19" s="62" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="C19" s="62" t="s">
         <v>171</v>
@@ -5743,7 +5749,7 @@
         <v>129</v>
       </c>
       <c r="B20" s="62" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="C20" s="52" t="s">
         <v>173</v>
@@ -5759,7 +5765,7 @@
         <v>129</v>
       </c>
       <c r="B21" s="62" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="C21" s="52" t="s">
         <v>175</v>
@@ -5775,7 +5781,7 @@
         <v>129</v>
       </c>
       <c r="B22" s="62" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="C22" s="52" t="s">
         <v>177</v>
@@ -5791,7 +5797,7 @@
         <v>129</v>
       </c>
       <c r="B23" s="62" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="C23" s="52" t="s">
         <v>167</v>
@@ -5842,7 +5848,7 @@
         <v>163</v>
       </c>
       <c r="C26" s="62" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="D26" s="63" t="s">
         <v>176</v>
@@ -5871,7 +5877,7 @@
         <v>129</v>
       </c>
       <c r="B28" s="52" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="C28" s="52" t="s">
         <v>183</v>
@@ -5887,7 +5893,7 @@
         <v>129</v>
       </c>
       <c r="B29" s="62" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="C29" s="52" t="s">
         <v>186</v>
@@ -5903,7 +5909,7 @@
         <v>129</v>
       </c>
       <c r="B30" s="62" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="C30" s="52" t="s">
         <v>135</v>
@@ -5919,7 +5925,7 @@
         <v>129</v>
       </c>
       <c r="B31" s="62" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="C31" s="52" t="s">
         <v>138</v>
@@ -5935,7 +5941,7 @@
         <v>129</v>
       </c>
       <c r="B32" s="62" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="C32" s="52" t="s">
         <v>140</v>
@@ -5967,7 +5973,7 @@
         <v>129</v>
       </c>
       <c r="B34" s="62" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="C34" s="52" t="s">
         <v>189</v>
@@ -5983,7 +5989,7 @@
         <v>129</v>
       </c>
       <c r="B35" s="62" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="C35" s="52" t="s">
         <v>191</v>
@@ -5999,7 +6005,7 @@
         <v>129</v>
       </c>
       <c r="B36" s="62" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="C36" s="52" t="s">
         <v>193</v>
@@ -6015,7 +6021,7 @@
         <v>129</v>
       </c>
       <c r="B37" s="62" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="C37" s="52" t="s">
         <v>195</v>
@@ -6031,7 +6037,7 @@
         <v>129</v>
       </c>
       <c r="B38" s="62" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C38" s="52" t="s">
         <v>183</v>
@@ -6047,7 +6053,7 @@
         <v>129</v>
       </c>
       <c r="B39" s="62" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="C39" s="52" t="s">
         <v>197</v>
@@ -6063,7 +6069,7 @@
         <v>129</v>
       </c>
       <c r="B40" s="62" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="C40" s="52" t="s">
         <v>135</v>
@@ -6079,7 +6085,7 @@
         <v>129</v>
       </c>
       <c r="B41" s="62" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="C41" s="52" t="s">
         <v>138</v>
@@ -6095,7 +6101,7 @@
         <v>129</v>
       </c>
       <c r="B42" s="62" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="C42" s="52" t="s">
         <v>140</v>
@@ -6191,7 +6197,7 @@
         <v>129</v>
       </c>
       <c r="B48" s="62" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="C48" s="52" t="s">
         <v>207</v>
@@ -6207,7 +6213,7 @@
         <v>129</v>
       </c>
       <c r="B49" s="62" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="C49" s="52" t="s">
         <v>135</v>
@@ -6223,7 +6229,7 @@
         <v>129</v>
       </c>
       <c r="B50" s="62" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="C50" s="52" t="s">
         <v>138</v>
@@ -6239,7 +6245,7 @@
         <v>129</v>
       </c>
       <c r="B51" s="62" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="C51" s="52" t="s">
         <v>140</v>
@@ -6255,7 +6261,7 @@
         <v>129</v>
       </c>
       <c r="B52" s="62" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="C52" s="52" t="s">
         <v>208</v>
@@ -6271,7 +6277,7 @@
         <v>129</v>
       </c>
       <c r="B53" s="62" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="C53" s="52" t="s">
         <v>210</v>
@@ -6287,7 +6293,7 @@
         <v>129</v>
       </c>
       <c r="B54" s="62" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="C54" s="52" t="s">
         <v>212</v>
@@ -6303,7 +6309,7 @@
         <v>129</v>
       </c>
       <c r="B55" s="62" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="C55" s="52" t="s">
         <v>214</v>
@@ -6319,7 +6325,7 @@
         <v>129</v>
       </c>
       <c r="B56" s="62" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="C56" s="52" t="s">
         <v>216</v>
@@ -6335,7 +6341,7 @@
         <v>129</v>
       </c>
       <c r="B57" s="62" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="C57" s="52" t="s">
         <v>183</v>
@@ -6351,7 +6357,7 @@
         <v>129</v>
       </c>
       <c r="B58" s="62" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="C58" s="52" t="s">
         <v>218</v>
@@ -6367,7 +6373,7 @@
         <v>129</v>
       </c>
       <c r="B59" s="62" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="C59" s="52" t="s">
         <v>135</v>
@@ -6383,7 +6389,7 @@
         <v>129</v>
       </c>
       <c r="B60" s="62" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="C60" s="52" t="s">
         <v>138</v>
@@ -6399,7 +6405,7 @@
         <v>129</v>
       </c>
       <c r="B61" s="62" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="C61" s="52" t="s">
         <v>140</v>
@@ -6415,7 +6421,7 @@
         <v>129</v>
       </c>
       <c r="B62" s="62" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="C62" s="52" t="s">
         <v>219</v>
@@ -6431,7 +6437,7 @@
         <v>129</v>
       </c>
       <c r="B63" s="62" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="C63" s="52" t="s">
         <v>221</v>
@@ -6447,7 +6453,7 @@
         <v>129</v>
       </c>
       <c r="B64" s="62" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="C64" s="52" t="s">
         <v>223</v>
@@ -6463,7 +6469,7 @@
         <v>129</v>
       </c>
       <c r="B65" s="62" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="C65" s="52" t="s">
         <v>183</v>
@@ -6479,7 +6485,7 @@
         <v>129</v>
       </c>
       <c r="B66" s="62" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="C66" s="52" t="s">
         <v>225</v>
@@ -6497,7 +6503,7 @@
         <v>129</v>
       </c>
       <c r="B67" s="62" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="C67" s="52" t="s">
         <v>135</v>
@@ -6513,7 +6519,7 @@
         <v>129</v>
       </c>
       <c r="B68" s="62" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="C68" s="52" t="s">
         <v>138</v>
@@ -6529,7 +6535,7 @@
         <v>129</v>
       </c>
       <c r="B69" s="62" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="C69" s="52" t="s">
         <v>140</v>
@@ -6545,7 +6551,7 @@
         <v>129</v>
       </c>
       <c r="B70" s="62" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="C70" s="52" t="s">
         <v>187</v>
@@ -6561,7 +6567,7 @@
         <v>129</v>
       </c>
       <c r="B71" s="62" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="C71" s="52" t="s">
         <v>189</v>
@@ -6577,7 +6583,7 @@
         <v>129</v>
       </c>
       <c r="B72" s="62" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="C72" s="52" t="s">
         <v>191</v>
@@ -6593,7 +6599,7 @@
         <v>129</v>
       </c>
       <c r="B73" s="62" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="C73" s="52" t="s">
         <v>195</v>
@@ -6609,7 +6615,7 @@
         <v>129</v>
       </c>
       <c r="B74" s="62" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="C74" s="52" t="s">
         <v>193</v>
@@ -6625,7 +6631,7 @@
         <v>129</v>
       </c>
       <c r="B75" s="62" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="C75" s="52" t="s">
         <v>183</v>
@@ -6641,7 +6647,7 @@
         <v>129</v>
       </c>
       <c r="B76" s="62" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="C76" s="52" t="s">
         <v>226</v>
@@ -6659,7 +6665,7 @@
         <v>129</v>
       </c>
       <c r="B77" s="62" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="C77" s="52" t="s">
         <v>135</v>
@@ -6675,7 +6681,7 @@
         <v>129</v>
       </c>
       <c r="B78" s="62" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="C78" s="52" t="s">
         <v>138</v>
@@ -6691,7 +6697,7 @@
         <v>129</v>
       </c>
       <c r="B79" s="62" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="C79" s="52" t="s">
         <v>140</v>
@@ -6707,7 +6713,7 @@
         <v>129</v>
       </c>
       <c r="B80" s="62" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="C80" s="52" t="s">
         <v>187</v>
@@ -6723,7 +6729,7 @@
         <v>129</v>
       </c>
       <c r="B81" s="62" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="C81" s="52" t="s">
         <v>189</v>
@@ -6739,7 +6745,7 @@
         <v>129</v>
       </c>
       <c r="B82" s="62" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="C82" s="52" t="s">
         <v>191</v>
@@ -6755,7 +6761,7 @@
         <v>129</v>
       </c>
       <c r="B83" s="62" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="C83" s="52" t="s">
         <v>193</v>
@@ -6771,7 +6777,7 @@
         <v>129</v>
       </c>
       <c r="B84" s="62" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="C84" s="52" t="s">
         <v>195</v>
@@ -6787,7 +6793,7 @@
         <v>129</v>
       </c>
       <c r="B85" s="62" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="C85" s="52" t="s">
         <v>183</v>
@@ -6803,7 +6809,7 @@
         <v>129</v>
       </c>
       <c r="B86" s="62" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="C86" s="52" t="s">
         <v>227</v>
@@ -6821,7 +6827,7 @@
         <v>129</v>
       </c>
       <c r="B87" s="62" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="C87" s="52" t="s">
         <v>135</v>
@@ -6837,7 +6843,7 @@
         <v>129</v>
       </c>
       <c r="B88" s="62" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="C88" s="52" t="s">
         <v>138</v>
@@ -6853,7 +6859,7 @@
         <v>129</v>
       </c>
       <c r="B89" s="62" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="C89" s="52" t="s">
         <v>140</v>
@@ -6869,7 +6875,7 @@
         <v>129</v>
       </c>
       <c r="B90" s="62" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="C90" s="52" t="s">
         <v>187</v>
@@ -6885,7 +6891,7 @@
         <v>129</v>
       </c>
       <c r="B91" s="62" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="C91" s="52" t="s">
         <v>189</v>
@@ -6901,7 +6907,7 @@
         <v>129</v>
       </c>
       <c r="B92" s="62" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="C92" s="52" t="s">
         <v>191</v>
@@ -6917,7 +6923,7 @@
         <v>129</v>
       </c>
       <c r="B93" s="62" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="C93" s="52" t="s">
         <v>193</v>
@@ -6933,7 +6939,7 @@
         <v>129</v>
       </c>
       <c r="B94" s="62" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="C94" s="52" t="s">
         <v>195</v>
@@ -6949,7 +6955,7 @@
         <v>129</v>
       </c>
       <c r="B95" s="62" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="C95" s="52" t="s">
         <v>183</v>
@@ -6965,7 +6971,7 @@
         <v>129</v>
       </c>
       <c r="B96" s="62" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="C96" s="52" t="s">
         <v>228</v>
@@ -6983,7 +6989,7 @@
         <v>129</v>
       </c>
       <c r="B97" s="62" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="C97" s="52" t="s">
         <v>135</v>
@@ -6999,7 +7005,7 @@
         <v>129</v>
       </c>
       <c r="B98" s="62" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="C98" s="52" t="s">
         <v>138</v>
@@ -7015,7 +7021,7 @@
         <v>129</v>
       </c>
       <c r="B99" s="62" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="C99" s="52" t="s">
         <v>140</v>
@@ -7031,7 +7037,7 @@
         <v>129</v>
       </c>
       <c r="B100" s="62" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="C100" s="52" t="s">
         <v>229</v>
@@ -7047,7 +7053,7 @@
         <v>129</v>
       </c>
       <c r="B101" s="62" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="C101" s="52" t="s">
         <v>231</v>
@@ -7063,7 +7069,7 @@
         <v>129</v>
       </c>
       <c r="B102" s="62" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="C102" s="52" t="s">
         <v>233</v>
@@ -7079,7 +7085,7 @@
         <v>129</v>
       </c>
       <c r="B103" s="62" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="C103" s="52" t="s">
         <v>235</v>
@@ -8198,7 +8204,7 @@
         <v>360</v>
       </c>
       <c r="C168" s="52" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="D168" s="52" t="s">
         <v>361</v>
@@ -8728,7 +8734,7 @@
         <v>442</v>
       </c>
       <c r="C201" s="52" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="D201" s="52" t="s">
         <v>412</v>
@@ -9048,7 +9054,7 @@
         <v>475</v>
       </c>
       <c r="C221" s="52" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="D221" s="52" t="s">
         <v>412</v>
@@ -10308,8 +10314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C15" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10319,7 +10325,7 @@
     <col min="3" max="3" width="23.875" style="64" customWidth="1"/>
     <col min="4" max="4" width="100" style="64" customWidth="1"/>
     <col min="5" max="6" width="22.875" style="64" customWidth="1"/>
-    <col min="7" max="7" width="10.5" style="64" customWidth="1"/>
+    <col min="7" max="7" width="20" style="64" customWidth="1"/>
     <col min="8" max="256" width="8.875" style="64" customWidth="1"/>
     <col min="257" max="16384" width="8.875" style="64"/>
   </cols>
@@ -10377,7 +10383,7 @@
         <v>641</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="E3" s="16"/>
       <c r="F3" s="16" t="s">
@@ -10433,8 +10439,8 @@
       <c r="C6" s="65" t="s">
         <v>644</v>
       </c>
-      <c r="D6" s="65" t="s">
-        <v>151</v>
+      <c r="D6" s="70" t="s">
+        <v>982</v>
       </c>
       <c r="E6" s="16"/>
       <c r="F6" s="16" t="s">
@@ -10442,7 +10448,7 @@
       </c>
       <c r="G6" s="16"/>
     </row>
-    <row r="7" spans="1:7" ht="126" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="66" t="s">
         <v>155</v>
       </c>
@@ -10459,9 +10465,7 @@
       <c r="F7" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="G7" s="16" t="s">
-        <v>634</v>
-      </c>
+      <c r="G7" s="16"/>
     </row>
     <row r="8" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="68" t="s">
@@ -11034,7 +11038,7 @@
         <v>133</v>
       </c>
       <c r="G37" s="69" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
     </row>
   </sheetData>
@@ -11050,8 +11054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:IV51"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11440,7 +11444,7 @@
         <v>717</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="E20" s="22"/>
       <c r="F20" s="2" t="s">
@@ -11820,7 +11824,7 @@
         <v>759</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>760</v>
+        <v>983</v>
       </c>
       <c r="E40" s="18"/>
       <c r="F40" s="3"/>
@@ -11834,10 +11838,10 @@
         <v>691</v>
       </c>
       <c r="C41" s="17" t="s">
+        <v>760</v>
+      </c>
+      <c r="D41" s="14" t="s">
         <v>761</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>762</v>
       </c>
       <c r="E41" s="18"/>
       <c r="F41" s="3"/>
@@ -11851,13 +11855,13 @@
         <v>691</v>
       </c>
       <c r="C42" s="17" t="s">
+        <v>762</v>
+      </c>
+      <c r="D42" s="14" t="s">
         <v>763</v>
       </c>
-      <c r="D42" s="14" t="s">
+      <c r="E42" s="14" t="s">
         <v>764</v>
-      </c>
-      <c r="E42" s="14" t="s">
-        <v>765</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
@@ -11870,13 +11874,13 @@
         <v>691</v>
       </c>
       <c r="C43" s="17" t="s">
+        <v>765</v>
+      </c>
+      <c r="D43" s="14" t="s">
         <v>766</v>
       </c>
-      <c r="D43" s="14" t="s">
+      <c r="E43" s="14" t="s">
         <v>767</v>
-      </c>
-      <c r="E43" s="14" t="s">
-        <v>768</v>
       </c>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
@@ -11889,13 +11893,13 @@
         <v>691</v>
       </c>
       <c r="C44" s="17" t="s">
+        <v>768</v>
+      </c>
+      <c r="D44" s="14" t="s">
         <v>769</v>
       </c>
-      <c r="D44" s="14" t="s">
+      <c r="E44" s="14" t="s">
         <v>770</v>
-      </c>
-      <c r="E44" s="14" t="s">
-        <v>771</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
@@ -11908,10 +11912,10 @@
         <v>691</v>
       </c>
       <c r="C45" s="17" t="s">
+        <v>771</v>
+      </c>
+      <c r="D45" s="14" t="s">
         <v>772</v>
-      </c>
-      <c r="D45" s="14" t="s">
-        <v>773</v>
       </c>
       <c r="E45" s="18"/>
       <c r="F45" s="3"/>
@@ -11925,10 +11929,10 @@
         <v>691</v>
       </c>
       <c r="C46" s="17" t="s">
+        <v>773</v>
+      </c>
+      <c r="D46" s="14" t="s">
         <v>774</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>775</v>
       </c>
       <c r="E46" s="18"/>
       <c r="F46" s="3"/>
@@ -11942,10 +11946,10 @@
         <v>691</v>
       </c>
       <c r="C47" s="17" t="s">
+        <v>775</v>
+      </c>
+      <c r="D47" s="14" t="s">
         <v>776</v>
-      </c>
-      <c r="D47" s="14" t="s">
-        <v>777</v>
       </c>
       <c r="E47" s="18"/>
       <c r="F47" s="3"/>
@@ -11953,16 +11957,16 @@
     </row>
     <row r="48" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B48" s="17" t="s">
         <v>691</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>780</v>
+        <v>984</v>
       </c>
       <c r="E48" s="18"/>
       <c r="F48" s="3"/>
@@ -11970,16 +11974,16 @@
     </row>
     <row r="49" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="B49" s="17" t="s">
         <v>691</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="E49" s="18"/>
       <c r="F49" s="3"/>
@@ -11987,16 +11991,16 @@
     </row>
     <row r="50" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="B50" s="17" t="s">
         <v>691</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="E50" s="18"/>
       <c r="F50" s="3"/>
@@ -12004,19 +12008,19 @@
     </row>
     <row r="51" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B51" s="17" t="s">
         <v>691</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="E51" s="14" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
@@ -12078,13 +12082,13 @@
         <v>388</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>788</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>789</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>790</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>791</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>792</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="14" t="s">
@@ -12097,13 +12101,13 @@
         <v>391</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="14" t="s">
@@ -12116,13 +12120,13 @@
         <v>394</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="14" t="s">
@@ -12135,13 +12139,13 @@
         <v>409</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="14" t="s">
@@ -12154,13 +12158,13 @@
         <v>397</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="14" t="s">
@@ -12173,13 +12177,13 @@
         <v>400</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="14" t="s">
@@ -12192,13 +12196,13 @@
         <v>403</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="14" t="s">
@@ -12211,13 +12215,13 @@
         <v>406</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="14" t="s">
@@ -12230,13 +12234,13 @@
         <v>412</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="14" t="s">
@@ -12246,16 +12250,16 @@
     </row>
     <row r="11" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
+        <v>806</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>788</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>807</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>808</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>790</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>809</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>810</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="14" t="s">
@@ -12268,13 +12272,13 @@
         <v>415</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="E12" s="26"/>
       <c r="F12" s="14" t="s">
@@ -12287,22 +12291,22 @@
         <v>418</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C13" s="20" t="s">
+        <v>811</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>812</v>
+      </c>
+      <c r="E13" s="28" t="s">
         <v>813</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="F13" s="29" t="s">
+        <v>240</v>
+      </c>
+      <c r="G13" s="14" t="s">
         <v>814</v>
-      </c>
-      <c r="E13" s="28" t="s">
-        <v>815</v>
-      </c>
-      <c r="F13" s="29" t="s">
-        <v>240</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>816</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -12310,13 +12314,13 @@
         <v>421</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="E14" s="30"/>
       <c r="F14" s="14" t="s">
@@ -12329,22 +12333,22 @@
         <v>424</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>456</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="F15" s="14" t="s">
         <v>240</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12352,13 +12356,13 @@
         <v>450</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="E16" s="14"/>
       <c r="F16" s="14" t="s">
@@ -12371,22 +12375,22 @@
         <v>459</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>458</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="F17" s="14" t="s">
         <v>240</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -12394,10 +12398,10 @@
         <v>490</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>489</v>
@@ -12413,10 +12417,10 @@
         <v>493</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>492</v>
@@ -12432,13 +12436,13 @@
         <v>496</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="14" t="s">
@@ -12451,13 +12455,13 @@
         <v>499</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="14" t="s">
@@ -12470,13 +12474,13 @@
         <v>504</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="E22" s="15"/>
       <c r="F22" s="14" t="s">
@@ -12489,10 +12493,10 @@
         <v>444</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>501</v>
@@ -12554,16 +12558,16 @@
         <v>427</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>834</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>835</v>
+      </c>
+      <c r="D2" s="33" t="s">
         <v>836</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="E2" s="34" t="s">
         <v>837</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>838</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>839</v>
       </c>
       <c r="F2" s="35" t="s">
         <v>240</v>
@@ -12575,16 +12579,16 @@
         <v>464</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="E3" s="34" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="F3" s="35" t="s">
         <v>240</v>
@@ -12596,16 +12600,16 @@
         <v>447</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="E4" s="36" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="F4" s="35" t="s">
         <v>240</v>
@@ -12722,20 +12726,20 @@
         <v>507</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>842</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>843</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>844</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>845</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>846</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="14" t="s">
         <v>240</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -12743,13 +12747,13 @@
         <v>559</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="14" t="s">
@@ -12762,10 +12766,10 @@
         <v>516</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>515</v>
@@ -12781,10 +12785,10 @@
         <v>519</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>518</v>
@@ -12800,10 +12804,10 @@
         <v>522</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>521</v>
@@ -12819,22 +12823,22 @@
         <v>525</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="D7" s="42" t="s">
         <v>524</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="F7" s="29" t="s">
         <v>240</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -12842,13 +12846,13 @@
         <v>528</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="E8" s="43"/>
       <c r="F8" s="14" t="s">
@@ -12861,13 +12865,13 @@
         <v>531</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="E9" s="40"/>
       <c r="F9" s="14" t="s">
@@ -12880,13 +12884,13 @@
         <v>534</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="E10" s="40"/>
       <c r="F10" s="14" t="s">
@@ -12899,10 +12903,10 @@
         <v>537</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>536</v>
@@ -12918,10 +12922,10 @@
         <v>540</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>539</v>
@@ -12937,22 +12941,22 @@
         <v>543</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C13" s="14" t="s">
+        <v>862</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>863</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>823</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>240</v>
+      </c>
+      <c r="G13" s="14" t="s">
         <v>864</v>
-      </c>
-      <c r="D13" s="42" t="s">
-        <v>865</v>
-      </c>
-      <c r="E13" s="28" t="s">
-        <v>825</v>
-      </c>
-      <c r="F13" s="29" t="s">
-        <v>240</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>866</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -12960,22 +12964,22 @@
         <v>550</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="D14" s="42" t="s">
         <v>549</v>
       </c>
       <c r="E14" s="28" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="F14" s="29" t="s">
         <v>240</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -12983,10 +12987,10 @@
         <v>553</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>552</v>
@@ -13002,13 +13006,13 @@
         <v>562</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="E16" s="40"/>
       <c r="F16" s="14" t="s">
@@ -13021,13 +13025,13 @@
         <v>579</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="E17" s="40"/>
       <c r="F17" s="14" t="s">
@@ -13040,13 +13044,13 @@
         <v>565</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="E18" s="41"/>
       <c r="F18" s="14" t="s">
@@ -13059,22 +13063,22 @@
         <v>600</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C19" s="14" t="s">
+        <v>875</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>876</v>
+      </c>
+      <c r="E19" s="28" t="s">
         <v>877</v>
       </c>
-      <c r="D19" s="42" t="s">
+      <c r="F19" s="29" t="s">
+        <v>240</v>
+      </c>
+      <c r="G19" s="14" t="s">
         <v>878</v>
-      </c>
-      <c r="E19" s="28" t="s">
-        <v>879</v>
-      </c>
-      <c r="F19" s="29" t="s">
-        <v>240</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>880</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -13082,13 +13086,13 @@
         <v>603</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="E20" s="44"/>
       <c r="F20" s="14" t="s">
@@ -13101,22 +13105,22 @@
         <v>606</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C21" s="32" t="s">
+        <v>881</v>
+      </c>
+      <c r="D21" s="45" t="s">
+        <v>882</v>
+      </c>
+      <c r="E21" s="28" t="s">
         <v>883</v>
       </c>
-      <c r="D21" s="45" t="s">
+      <c r="F21" s="46" t="s">
+        <v>240</v>
+      </c>
+      <c r="G21" s="32" t="s">
         <v>884</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>885</v>
-      </c>
-      <c r="F21" s="46" t="s">
-        <v>240</v>
-      </c>
-      <c r="G21" s="32" t="s">
-        <v>886</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -13124,22 +13128,22 @@
         <v>621</v>
       </c>
       <c r="B22" s="48" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C22" s="49" t="s">
+        <v>885</v>
+      </c>
+      <c r="D22" s="49" t="s">
+        <v>886</v>
+      </c>
+      <c r="E22" s="49" t="s">
         <v>887</v>
-      </c>
-      <c r="D22" s="49" t="s">
-        <v>888</v>
-      </c>
-      <c r="E22" s="49" t="s">
-        <v>889</v>
       </c>
       <c r="F22" s="49" t="s">
         <v>133</v>
       </c>
       <c r="G22" s="50" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
     </row>
   </sheetData>
@@ -13169,7 +13173,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>126</v>
@@ -13249,7 +13253,7 @@
         <v>144</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
@@ -14153,7 +14157,7 @@
     </row>
     <row r="101" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="14" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="B101" s="15"/>
       <c r="C101" s="15"/>
@@ -14162,7 +14166,7 @@
     </row>
     <row r="102" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="14" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="B102" s="15"/>
       <c r="C102" s="15"/>

</xml_diff>

<commit_message>
Last try before learning python
</commit_message>
<xml_diff>
--- a/docs/coverage-testing/85b_test_definitions_PIV_ICAM_Test_Cards_Exploded.xlsx
+++ b/docs/coverage-testing/85b_test_definitions_PIV_ICAM_Test_Cards_Exploded.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\docs\coverage-testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499423AD-1334-4AFD-9D78-F4255078D911}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF88D7A-AFE6-4B12-A4E7-E4DE159DC577}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2775" yWindow="255" windowWidth="27930" windowHeight="15240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2253" uniqueCount="986">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2253" uniqueCount="985">
   <si>
     <t>Test Case</t>
   </si>
@@ -2995,9 +2995,6 @@
   </si>
   <si>
     <t>Validate that the Reserved for Future Use field is equal to 0x00000000</t>
-  </si>
-  <si>
-    <t>Validate that the “Reserved for Future Use field is equal to 0x00000000</t>
   </si>
   <si>
     <t>The accessLocation for this AccessMethod is of type uniformResourceIdentifier and that the scheme is “http (not “https).</t>
@@ -5403,8 +5400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F287"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="C146" sqref="C146"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7349,7 +7346,7 @@
         <v>281</v>
       </c>
       <c r="C119" s="60" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="D119" s="50" t="s">
         <v>282</v>
@@ -9469,7 +9466,7 @@
         <v>527</v>
       </c>
       <c r="C248" s="50" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="D248" s="50" t="s">
         <v>528</v>

</xml_diff>

<commit_message>
Killed last 2 hiding around http
</commit_message>
<xml_diff>
--- a/docs/coverage-testing/85b_test_definitions_PIV_ICAM_Test_Cards_Exploded.xlsx
+++ b/docs/coverage-testing/85b_test_definitions_PIV_ICAM_Test_Cards_Exploded.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\docs\coverage-testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF88D7A-AFE6-4B12-A4E7-E4DE159DC577}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95ABAFCE-D3B1-40DD-8350-088DA52F9324}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2775" yWindow="255" windowWidth="27930" windowHeight="15240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2997,7 +2997,7 @@
     <t>Validate that the Reserved for Future Use field is equal to 0x00000000</t>
   </si>
   <si>
-    <t>The accessLocation for this AccessMethod is of type uniformResourceIdentifier and that the scheme is “http (not “https).</t>
+    <t>The accessLocation for this AccessMethod is of type uniformResourceIdentifier and that the scheme is http (not https).</t>
   </si>
 </sst>
 </file>
@@ -5400,8 +5400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F287"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="C135" sqref="C135"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A252" workbookViewId="0">
+      <selection activeCell="C251" sqref="C251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added to test coverage directory
</commit_message>
<xml_diff>
--- a/docs/coverage-testing/85b_test_definitions_PIV_ICAM_Test_Cards_Exploded.xlsx
+++ b/docs/coverage-testing/85b_test_definitions_PIV_ICAM_Test_Cards_Exploded.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\docs\coverage-testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95ABAFCE-D3B1-40DD-8350-088DA52F9324}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEACE89-2F93-439F-BFD7-700321AEE4F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2775" yWindow="255" windowWidth="27930" windowHeight="15240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2490" yWindow="75" windowWidth="27930" windowHeight="15240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIV I Reference Tests" sheetId="1" r:id="rId1"/>
@@ -5400,8 +5400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F287"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A252" workbookViewId="0">
-      <selection activeCell="C251" sqref="C251"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="D285" sqref="D285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -12664,8 +12664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:IV22"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Moved 0xdeadbeef to column D.
</commit_message>
<xml_diff>
--- a/docs/coverage-testing/85b_test_definitions_PIV_ICAM_Test_Cards_Exploded.xlsx
+++ b/docs/coverage-testing/85b_test_definitions_PIV_ICAM_Test_Cards_Exploded.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\docs\coverage-testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA43BF18-1280-4A63-B0F7-5FE67B1E1AE8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09C2153-5F2C-4C7E-8336-AB3AF05B6784}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="450" windowWidth="25680" windowHeight="16305" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="165" yWindow="450" windowWidth="25680" windowHeight="16305" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIV I Reference Tests" sheetId="1" r:id="rId1"/>
@@ -6080,10 +6080,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{539C8DD9-7E09-4AC9-B53E-1B766442D166}">
-  <dimension ref="A1:D449"/>
+  <dimension ref="A1:E449"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E422" sqref="E422:E427"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -6092,6 +6092,7 @@
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="85.375" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -7640,7 +7641,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:5">
       <c r="A113" s="62" t="s">
         <v>125</v>
       </c>
@@ -7654,7 +7655,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="31.5">
+    <row r="114" spans="1:5" ht="31.5">
       <c r="A114" s="62" t="s">
         <v>125</v>
       </c>
@@ -7668,7 +7669,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:5">
       <c r="A115" s="62" t="s">
         <v>125</v>
       </c>
@@ -7680,7 +7681,7 @@
       </c>
       <c r="D115" s="65"/>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:5">
       <c r="A116" s="62" t="s">
         <v>125</v>
       </c>
@@ -7690,11 +7691,11 @@
       <c r="C116" s="68" t="s">
         <v>931</v>
       </c>
-      <c r="D116" s="65" t="s">
+      <c r="E116" s="65" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:5">
       <c r="A117" s="62" t="s">
         <v>125</v>
       </c>
@@ -7704,11 +7705,11 @@
       <c r="C117" s="68" t="s">
         <v>130</v>
       </c>
-      <c r="D117" s="65" t="s">
+      <c r="E117" s="65" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:5">
       <c r="A118" s="62" t="s">
         <v>125</v>
       </c>
@@ -7718,11 +7719,11 @@
       <c r="C118" s="68" t="s">
         <v>133</v>
       </c>
-      <c r="D118" s="65" t="s">
+      <c r="E118" s="65" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:5">
       <c r="A119" s="62" t="s">
         <v>125</v>
       </c>
@@ -7732,11 +7733,11 @@
       <c r="C119" s="68" t="s">
         <v>135</v>
       </c>
-      <c r="D119" s="65" t="s">
+      <c r="E119" s="65" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:5">
       <c r="A120" s="62" t="s">
         <v>125</v>
       </c>
@@ -7746,11 +7747,11 @@
       <c r="C120" s="68" t="s">
         <v>937</v>
       </c>
-      <c r="D120" s="65" t="s">
+      <c r="E120" s="65" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="31.5">
+    <row r="121" spans="1:5" ht="31.5">
       <c r="A121" s="62" t="s">
         <v>125</v>
       </c>
@@ -7760,11 +7761,11 @@
       <c r="C121" s="69" t="s">
         <v>939</v>
       </c>
-      <c r="D121" s="65" t="s">
+      <c r="E121" s="65" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:5">
       <c r="A122" s="62" t="s">
         <v>125</v>
       </c>
@@ -7774,11 +7775,11 @@
       <c r="C122" s="69" t="s">
         <v>941</v>
       </c>
-      <c r="D122" s="65" t="s">
+      <c r="E122" s="65" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="47.25">
+    <row r="123" spans="1:5" ht="47.25">
       <c r="A123" s="62" t="s">
         <v>125</v>
       </c>
@@ -7788,11 +7789,11 @@
       <c r="C123" s="69" t="s">
         <v>943</v>
       </c>
-      <c r="D123" s="65" t="s">
+      <c r="E123" s="65" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:5">
       <c r="A124" s="62" t="s">
         <v>125</v>
       </c>
@@ -7802,11 +7803,11 @@
       <c r="C124" s="69" t="s">
         <v>945</v>
       </c>
-      <c r="D124" s="65" t="s">
+      <c r="E124" s="65" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:5">
       <c r="A125" s="62" t="s">
         <v>125</v>
       </c>
@@ -7816,11 +7817,11 @@
       <c r="C125" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="D125" s="65" t="s">
+      <c r="E125" s="65" t="s">
         <v>947</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:5">
       <c r="A126" s="62" t="s">
         <v>125</v>
       </c>
@@ -7832,7 +7833,7 @@
       </c>
       <c r="D126" s="65"/>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:5">
       <c r="A127" s="62" t="s">
         <v>125</v>
       </c>
@@ -7842,11 +7843,11 @@
       <c r="C127" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="D127" s="65" t="s">
+      <c r="E127" s="65" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:5">
       <c r="A128" s="62" t="s">
         <v>125</v>
       </c>
@@ -7856,11 +7857,11 @@
       <c r="C128" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="D128" s="65" t="s">
+      <c r="E128" s="65" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:5">
       <c r="A129" s="62" t="s">
         <v>125</v>
       </c>
@@ -7870,11 +7871,11 @@
       <c r="C129" s="69" t="s">
         <v>952</v>
       </c>
-      <c r="D129" s="65" t="s">
+      <c r="E129" s="65" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:5">
       <c r="A130" s="62" t="s">
         <v>125</v>
       </c>
@@ -7884,11 +7885,11 @@
       <c r="C130" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="D130" s="65" t="s">
+      <c r="E130" s="65" t="s">
         <v>947</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:5">
       <c r="A131" s="62" t="s">
         <v>125</v>
       </c>
@@ -7898,11 +7899,11 @@
       <c r="C131" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="D131" s="65" t="s">
+      <c r="E131" s="65" t="s">
         <v>947</v>
       </c>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:5">
       <c r="A132" s="62" t="s">
         <v>125</v>
       </c>
@@ -7912,11 +7913,11 @@
       <c r="C132" s="70" t="s">
         <v>41</v>
       </c>
-      <c r="D132" s="65" t="s">
+      <c r="E132" s="65" t="s">
         <v>947</v>
       </c>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:5">
       <c r="A133" s="58" t="s">
         <v>125</v>
       </c>
@@ -7928,7 +7929,7 @@
       </c>
       <c r="D133" s="61"/>
     </row>
-    <row r="134" spans="1:4">
+    <row r="134" spans="1:5">
       <c r="A134" s="62" t="s">
         <v>125</v>
       </c>
@@ -7940,7 +7941,7 @@
       </c>
       <c r="D134" s="65"/>
     </row>
-    <row r="135" spans="1:4">
+    <row r="135" spans="1:5">
       <c r="A135" s="62" t="s">
         <v>125</v>
       </c>
@@ -7952,7 +7953,7 @@
       </c>
       <c r="D135" s="65"/>
     </row>
-    <row r="136" spans="1:4">
+    <row r="136" spans="1:5">
       <c r="A136" s="62" t="s">
         <v>125</v>
       </c>
@@ -7966,7 +7967,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="137" spans="1:4">
+    <row r="137" spans="1:5">
       <c r="A137" s="62" t="s">
         <v>125</v>
       </c>
@@ -7980,7 +7981,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:5">
       <c r="A138" s="62" t="s">
         <v>125</v>
       </c>
@@ -7994,7 +7995,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:5">
       <c r="A139" s="62" t="s">
         <v>125</v>
       </c>
@@ -8008,7 +8009,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" spans="1:5">
       <c r="A140" s="62" t="s">
         <v>125</v>
       </c>
@@ -8020,7 +8021,7 @@
       </c>
       <c r="D140" s="65"/>
     </row>
-    <row r="141" spans="1:4">
+    <row r="141" spans="1:5">
       <c r="A141" s="62" t="s">
         <v>125</v>
       </c>
@@ -8034,7 +8035,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="142" spans="1:4">
+    <row r="142" spans="1:5">
       <c r="A142" s="62" t="s">
         <v>125</v>
       </c>
@@ -8048,7 +8049,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="31.5">
+    <row r="143" spans="1:5" ht="31.5">
       <c r="A143" s="62" t="s">
         <v>125</v>
       </c>
@@ -8062,7 +8063,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="31.5">
+    <row r="144" spans="1:5" ht="31.5">
       <c r="A144" s="62" t="s">
         <v>125</v>
       </c>
@@ -8954,7 +8955,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="209" spans="1:4">
+    <row r="209" spans="1:5">
       <c r="A209" s="62" t="s">
         <v>125</v>
       </c>
@@ -8968,7 +8969,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="210" spans="1:4">
+    <row r="210" spans="1:5">
       <c r="A210" s="62" t="s">
         <v>125</v>
       </c>
@@ -8982,7 +8983,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="211" spans="1:4">
+    <row r="211" spans="1:5">
       <c r="A211" s="62" t="s">
         <v>125</v>
       </c>
@@ -8992,11 +8993,11 @@
       <c r="C211" s="63" t="s">
         <v>974</v>
       </c>
-      <c r="D211" s="65" t="s">
+      <c r="E211" s="65" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="212" spans="1:4">
+    <row r="212" spans="1:5">
       <c r="A212" s="62" t="s">
         <v>125</v>
       </c>
@@ -9010,7 +9011,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="213" spans="1:4">
+    <row r="213" spans="1:5">
       <c r="A213" s="62" t="s">
         <v>125</v>
       </c>
@@ -9024,7 +9025,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="214" spans="1:4">
+    <row r="214" spans="1:5">
       <c r="A214" s="62" t="s">
         <v>125</v>
       </c>
@@ -9038,7 +9039,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="215" spans="1:4">
+    <row r="215" spans="1:5">
       <c r="A215" s="62" t="s">
         <v>125</v>
       </c>
@@ -9052,7 +9053,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="216" spans="1:4">
+    <row r="216" spans="1:5">
       <c r="A216" s="62" t="s">
         <v>125</v>
       </c>
@@ -9066,7 +9067,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="217" spans="1:4">
+    <row r="217" spans="1:5">
       <c r="A217" s="62" t="s">
         <v>125</v>
       </c>
@@ -9080,7 +9081,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="218" spans="1:4">
+    <row r="218" spans="1:5">
       <c r="A218" s="62" t="s">
         <v>125</v>
       </c>
@@ -9092,7 +9093,7 @@
       </c>
       <c r="D218" s="65"/>
     </row>
-    <row r="219" spans="1:4">
+    <row r="219" spans="1:5">
       <c r="A219" s="62" t="s">
         <v>125</v>
       </c>
@@ -9106,7 +9107,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="220" spans="1:4">
+    <row r="220" spans="1:5">
       <c r="A220" s="62" t="s">
         <v>125</v>
       </c>
@@ -9120,7 +9121,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="221" spans="1:4">
+    <row r="221" spans="1:5">
       <c r="A221" s="62" t="s">
         <v>125</v>
       </c>
@@ -9132,7 +9133,7 @@
       </c>
       <c r="D221" s="65"/>
     </row>
-    <row r="222" spans="1:4">
+    <row r="222" spans="1:5">
       <c r="A222" s="62" t="s">
         <v>125</v>
       </c>
@@ -9142,11 +9143,11 @@
       <c r="C222" s="72" t="s">
         <v>984</v>
       </c>
-      <c r="D222" s="65" t="s">
+      <c r="E222" s="65" t="s">
         <v>947</v>
       </c>
     </row>
-    <row r="223" spans="1:4">
+    <row r="223" spans="1:5">
       <c r="A223" s="62" t="s">
         <v>125</v>
       </c>
@@ -9156,9 +9157,9 @@
       <c r="C223" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="D223" s="65"/>
-    </row>
-    <row r="224" spans="1:4">
+      <c r="E223" s="65"/>
+    </row>
+    <row r="224" spans="1:5">
       <c r="A224" s="62" t="s">
         <v>125</v>
       </c>
@@ -9168,11 +9169,11 @@
       <c r="C224" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="D224" s="65" t="s">
+      <c r="E224" s="65" t="s">
         <v>947</v>
       </c>
     </row>
-    <row r="225" spans="1:4">
+    <row r="225" spans="1:5">
       <c r="A225" s="62" t="s">
         <v>125</v>
       </c>
@@ -9182,11 +9183,11 @@
       <c r="C225" s="72" t="s">
         <v>67</v>
       </c>
-      <c r="D225" s="65" t="s">
+      <c r="E225" s="65" t="s">
         <v>947</v>
       </c>
     </row>
-    <row r="226" spans="1:4">
+    <row r="226" spans="1:5">
       <c r="A226" s="62" t="s">
         <v>125</v>
       </c>
@@ -9196,9 +9197,9 @@
       <c r="C226" s="64" t="s">
         <v>69</v>
       </c>
-      <c r="D226" s="65"/>
-    </row>
-    <row r="227" spans="1:4">
+      <c r="E226" s="65"/>
+    </row>
+    <row r="227" spans="1:5">
       <c r="A227" s="62" t="s">
         <v>125</v>
       </c>
@@ -9208,11 +9209,11 @@
       <c r="C227" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="D227" s="65" t="s">
+      <c r="E227" s="65" t="s">
         <v>947</v>
       </c>
     </row>
-    <row r="228" spans="1:4">
+    <row r="228" spans="1:5">
       <c r="A228" s="62" t="s">
         <v>125</v>
       </c>
@@ -9222,11 +9223,11 @@
       <c r="C228" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="D228" s="65" t="s">
+      <c r="E228" s="65" t="s">
         <v>947</v>
       </c>
     </row>
-    <row r="229" spans="1:4">
+    <row r="229" spans="1:5">
       <c r="A229" s="62" t="s">
         <v>125</v>
       </c>
@@ -9238,7 +9239,7 @@
       </c>
       <c r="D229" s="61"/>
     </row>
-    <row r="230" spans="1:4">
+    <row r="230" spans="1:5">
       <c r="A230" s="62" t="s">
         <v>125</v>
       </c>
@@ -9250,7 +9251,7 @@
       </c>
       <c r="D230" s="65"/>
     </row>
-    <row r="231" spans="1:4">
+    <row r="231" spans="1:5">
       <c r="A231" s="62" t="s">
         <v>125</v>
       </c>
@@ -9262,7 +9263,7 @@
       </c>
       <c r="D231" s="65"/>
     </row>
-    <row r="232" spans="1:4" ht="31.5">
+    <row r="232" spans="1:5" ht="31.5">
       <c r="A232" s="62" t="s">
         <v>125</v>
       </c>
@@ -9276,7 +9277,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="233" spans="1:4">
+    <row r="233" spans="1:5">
       <c r="A233" s="62" t="s">
         <v>125</v>
       </c>
@@ -9290,7 +9291,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="234" spans="1:4">
+    <row r="234" spans="1:5">
       <c r="A234" s="62" t="s">
         <v>125</v>
       </c>
@@ -9304,7 +9305,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="235" spans="1:4" ht="31.5">
+    <row r="235" spans="1:5" ht="31.5">
       <c r="A235" s="62" t="s">
         <v>125</v>
       </c>
@@ -9318,7 +9319,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="236" spans="1:4">
+    <row r="236" spans="1:5">
       <c r="A236" s="62" t="s">
         <v>125</v>
       </c>
@@ -9332,7 +9333,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="237" spans="1:4">
+    <row r="237" spans="1:5">
       <c r="A237" s="62" t="s">
         <v>125</v>
       </c>
@@ -9346,7 +9347,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="238" spans="1:4" ht="31.5">
+    <row r="238" spans="1:5" ht="31.5">
       <c r="A238" s="62" t="s">
         <v>125</v>
       </c>
@@ -9360,7 +9361,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="239" spans="1:4" ht="31.5">
+    <row r="239" spans="1:5" ht="31.5">
       <c r="A239" s="62" t="s">
         <v>125</v>
       </c>
@@ -9374,7 +9375,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="240" spans="1:4" ht="47.25">
+    <row r="240" spans="1:5" ht="47.25">
       <c r="A240" s="62" t="s">
         <v>125</v>
       </c>
@@ -10480,7 +10481,7 @@
       </c>
       <c r="D320" s="65"/>
     </row>
-    <row r="321" spans="1:4">
+    <row r="321" spans="1:5">
       <c r="A321" s="62" t="s">
         <v>125</v>
       </c>
@@ -10494,7 +10495,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="322" spans="1:4">
+    <row r="322" spans="1:5">
       <c r="A322" s="62" t="s">
         <v>125</v>
       </c>
@@ -10508,7 +10509,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="323" spans="1:4" ht="31.5">
+    <row r="323" spans="1:5" ht="31.5">
       <c r="A323" s="62" t="s">
         <v>125</v>
       </c>
@@ -10522,7 +10523,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="324" spans="1:4">
+    <row r="324" spans="1:5">
       <c r="A324" s="62" t="s">
         <v>125</v>
       </c>
@@ -10536,7 +10537,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="325" spans="1:4">
+    <row r="325" spans="1:5">
       <c r="A325" s="62" t="s">
         <v>125</v>
       </c>
@@ -10550,7 +10551,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="326" spans="1:4">
+    <row r="326" spans="1:5">
       <c r="A326" s="62" t="s">
         <v>125</v>
       </c>
@@ -10564,7 +10565,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="327" spans="1:4" ht="47.25">
+    <row r="327" spans="1:5" ht="47.25">
       <c r="A327" s="62" t="s">
         <v>125</v>
       </c>
@@ -10578,7 +10579,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="328" spans="1:4" ht="31.5">
+    <row r="328" spans="1:5" ht="31.5">
       <c r="A328" s="62" t="s">
         <v>125</v>
       </c>
@@ -10592,7 +10593,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="329" spans="1:4">
+    <row r="329" spans="1:5">
       <c r="A329" s="62" t="s">
         <v>125</v>
       </c>
@@ -10602,11 +10603,11 @@
       <c r="C329" s="69" t="s">
         <v>492</v>
       </c>
-      <c r="D329" s="65" t="s">
+      <c r="E329" s="65" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="330" spans="1:4" ht="31.5">
+    <row r="330" spans="1:5" ht="31.5">
       <c r="A330" s="62" t="s">
         <v>125</v>
       </c>
@@ -10620,7 +10621,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="331" spans="1:4">
+    <row r="331" spans="1:5">
       <c r="A331" s="62" t="s">
         <v>125</v>
       </c>
@@ -10634,7 +10635,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="332" spans="1:4">
+    <row r="332" spans="1:5">
       <c r="A332" s="62" t="s">
         <v>125</v>
       </c>
@@ -10646,7 +10647,7 @@
       </c>
       <c r="D332" s="65"/>
     </row>
-    <row r="333" spans="1:4">
+    <row r="333" spans="1:5">
       <c r="A333" s="62" t="s">
         <v>125</v>
       </c>
@@ -10660,7 +10661,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="334" spans="1:4">
+    <row r="334" spans="1:5">
       <c r="A334" s="62" t="s">
         <v>125</v>
       </c>
@@ -10670,11 +10671,11 @@
       <c r="C334" s="69" t="s">
         <v>1066</v>
       </c>
-      <c r="D334" s="65" t="s">
+      <c r="E334" s="65" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="335" spans="1:4">
+    <row r="335" spans="1:5">
       <c r="A335" s="62" t="s">
         <v>125</v>
       </c>
@@ -10686,7 +10687,7 @@
       </c>
       <c r="D335" s="65"/>
     </row>
-    <row r="336" spans="1:4">
+    <row r="336" spans="1:5">
       <c r="A336" s="62" t="s">
         <v>125</v>
       </c>
@@ -10700,7 +10701,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="337" spans="1:4">
+    <row r="337" spans="1:5">
       <c r="A337" s="62" t="s">
         <v>125</v>
       </c>
@@ -10714,7 +10715,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="338" spans="1:4">
+    <row r="338" spans="1:5">
       <c r="A338" s="62" t="s">
         <v>125</v>
       </c>
@@ -10728,7 +10729,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="339" spans="1:4">
+    <row r="339" spans="1:5">
       <c r="A339" s="62" t="s">
         <v>125</v>
       </c>
@@ -10742,7 +10743,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="340" spans="1:4">
+    <row r="340" spans="1:5">
       <c r="A340" s="62" t="s">
         <v>125</v>
       </c>
@@ -10752,11 +10753,11 @@
       <c r="C340" s="69" t="s">
         <v>1077</v>
       </c>
-      <c r="D340" s="65" t="s">
+      <c r="E340" s="65" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="341" spans="1:4">
+    <row r="341" spans="1:5">
       <c r="A341" s="62" t="s">
         <v>125</v>
       </c>
@@ -10768,7 +10769,7 @@
       </c>
       <c r="D341" s="65"/>
     </row>
-    <row r="342" spans="1:4">
+    <row r="342" spans="1:5">
       <c r="A342" s="62" t="s">
         <v>125</v>
       </c>
@@ -10780,7 +10781,7 @@
       </c>
       <c r="D342" s="65"/>
     </row>
-    <row r="343" spans="1:4" ht="63">
+    <row r="343" spans="1:5" ht="63">
       <c r="A343" s="62" t="s">
         <v>125</v>
       </c>
@@ -10794,7 +10795,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="344" spans="1:4">
+    <row r="344" spans="1:5">
       <c r="A344" s="62" t="s">
         <v>125</v>
       </c>
@@ -10808,7 +10809,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="345" spans="1:4">
+    <row r="345" spans="1:5">
       <c r="A345" s="62" t="s">
         <v>125</v>
       </c>
@@ -10822,7 +10823,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="346" spans="1:4">
+    <row r="346" spans="1:5">
       <c r="A346" s="62" t="s">
         <v>125</v>
       </c>
@@ -10834,7 +10835,7 @@
       </c>
       <c r="D346" s="65"/>
     </row>
-    <row r="347" spans="1:4">
+    <row r="347" spans="1:5">
       <c r="A347" s="62" t="s">
         <v>125</v>
       </c>
@@ -10846,7 +10847,7 @@
       </c>
       <c r="D347" s="65"/>
     </row>
-    <row r="348" spans="1:4">
+    <row r="348" spans="1:5">
       <c r="A348" s="62" t="s">
         <v>125</v>
       </c>
@@ -10860,7 +10861,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="349" spans="1:4">
+    <row r="349" spans="1:5">
       <c r="A349" s="62" t="s">
         <v>125</v>
       </c>
@@ -10874,7 +10875,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="350" spans="1:4" ht="31.5">
+    <row r="350" spans="1:5" ht="31.5">
       <c r="A350" s="62" t="s">
         <v>125</v>
       </c>
@@ -10888,7 +10889,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="351" spans="1:4" ht="31.5">
+    <row r="351" spans="1:5" ht="31.5">
       <c r="A351" s="62" t="s">
         <v>125</v>
       </c>
@@ -10902,7 +10903,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="352" spans="1:4">
+    <row r="352" spans="1:5">
       <c r="A352" s="62" t="s">
         <v>125</v>
       </c>
@@ -10916,7 +10917,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="353" spans="1:4" ht="31.5">
+    <row r="353" spans="1:5" ht="31.5">
       <c r="A353" s="62" t="s">
         <v>125</v>
       </c>
@@ -10930,7 +10931,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="354" spans="1:4">
+    <row r="354" spans="1:5">
       <c r="A354" s="62" t="s">
         <v>125</v>
       </c>
@@ -10942,7 +10943,7 @@
       </c>
       <c r="D354" s="65"/>
     </row>
-    <row r="355" spans="1:4">
+    <row r="355" spans="1:5">
       <c r="A355" s="62" t="s">
         <v>125</v>
       </c>
@@ -10956,7 +10957,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="356" spans="1:4">
+    <row r="356" spans="1:5">
       <c r="A356" s="62" t="s">
         <v>125</v>
       </c>
@@ -10966,11 +10967,11 @@
       <c r="C356" s="69" t="s">
         <v>1066</v>
       </c>
-      <c r="D356" s="65" t="s">
+      <c r="E356" s="65" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="357" spans="1:4">
+    <row r="357" spans="1:5">
       <c r="A357" s="62" t="s">
         <v>125</v>
       </c>
@@ -10982,7 +10983,7 @@
       </c>
       <c r="D357" s="65"/>
     </row>
-    <row r="358" spans="1:4">
+    <row r="358" spans="1:5">
       <c r="A358" s="62" t="s">
         <v>125</v>
       </c>
@@ -10996,7 +10997,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="359" spans="1:4">
+    <row r="359" spans="1:5">
       <c r="A359" s="62" t="s">
         <v>125</v>
       </c>
@@ -11010,7 +11011,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="360" spans="1:4">
+    <row r="360" spans="1:5">
       <c r="A360" s="62" t="s">
         <v>125</v>
       </c>
@@ -11024,7 +11025,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="361" spans="1:4">
+    <row r="361" spans="1:5">
       <c r="A361" s="62" t="s">
         <v>125</v>
       </c>
@@ -11038,7 +11039,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="362" spans="1:4">
+    <row r="362" spans="1:5">
       <c r="A362" s="62" t="s">
         <v>125</v>
       </c>
@@ -11048,11 +11049,11 @@
       <c r="C362" s="69" t="s">
         <v>1077</v>
       </c>
-      <c r="D362" s="65" t="s">
+      <c r="E362" s="65" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="363" spans="1:4">
+    <row r="363" spans="1:5">
       <c r="A363" s="62" t="s">
         <v>125</v>
       </c>
@@ -11064,7 +11065,7 @@
       </c>
       <c r="D363" s="65"/>
     </row>
-    <row r="364" spans="1:4">
+    <row r="364" spans="1:5">
       <c r="A364" s="62" t="s">
         <v>125</v>
       </c>
@@ -11076,7 +11077,7 @@
       </c>
       <c r="D364" s="65"/>
     </row>
-    <row r="365" spans="1:4" ht="47.25">
+    <row r="365" spans="1:5" ht="47.25">
       <c r="A365" s="62" t="s">
         <v>125</v>
       </c>
@@ -11090,7 +11091,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="366" spans="1:4">
+    <row r="366" spans="1:5">
       <c r="A366" s="62" t="s">
         <v>125</v>
       </c>
@@ -11104,7 +11105,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="367" spans="1:4">
+    <row r="367" spans="1:5">
       <c r="A367" s="62" t="s">
         <v>125</v>
       </c>
@@ -11118,7 +11119,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="368" spans="1:4">
+    <row r="368" spans="1:5">
       <c r="A368" s="62" t="s">
         <v>125</v>
       </c>
@@ -11130,7 +11131,7 @@
       </c>
       <c r="D368" s="65"/>
     </row>
-    <row r="369" spans="1:4">
+    <row r="369" spans="1:5">
       <c r="A369" s="62" t="s">
         <v>125</v>
       </c>
@@ -11142,7 +11143,7 @@
       </c>
       <c r="D369" s="65"/>
     </row>
-    <row r="370" spans="1:4">
+    <row r="370" spans="1:5">
       <c r="A370" s="62" t="s">
         <v>125</v>
       </c>
@@ -11156,7 +11157,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="371" spans="1:4">
+    <row r="371" spans="1:5">
       <c r="A371" s="62" t="s">
         <v>125</v>
       </c>
@@ -11170,7 +11171,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="372" spans="1:4">
+    <row r="372" spans="1:5">
       <c r="A372" s="62" t="s">
         <v>125</v>
       </c>
@@ -11184,7 +11185,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="373" spans="1:4" ht="31.5">
+    <row r="373" spans="1:5" ht="31.5">
       <c r="A373" s="62" t="s">
         <v>125</v>
       </c>
@@ -11198,7 +11199,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="374" spans="1:4">
+    <row r="374" spans="1:5">
       <c r="A374" s="62" t="s">
         <v>125</v>
       </c>
@@ -11212,7 +11213,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="375" spans="1:4" ht="31.5">
+    <row r="375" spans="1:5" ht="31.5">
       <c r="A375" s="62" t="s">
         <v>125</v>
       </c>
@@ -11226,7 +11227,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="376" spans="1:4">
+    <row r="376" spans="1:5">
       <c r="A376" s="62" t="s">
         <v>125</v>
       </c>
@@ -11238,7 +11239,7 @@
       </c>
       <c r="D376" s="65"/>
     </row>
-    <row r="377" spans="1:4">
+    <row r="377" spans="1:5">
       <c r="A377" s="62" t="s">
         <v>125</v>
       </c>
@@ -11252,7 +11253,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="378" spans="1:4">
+    <row r="378" spans="1:5">
       <c r="A378" s="62" t="s">
         <v>125</v>
       </c>
@@ -11262,11 +11263,11 @@
       <c r="C378" s="69" t="s">
         <v>1066</v>
       </c>
-      <c r="D378" s="65" t="s">
+      <c r="E378" s="65" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="379" spans="1:4">
+    <row r="379" spans="1:5">
       <c r="A379" s="62" t="s">
         <v>125</v>
       </c>
@@ -11278,7 +11279,7 @@
       </c>
       <c r="D379" s="65"/>
     </row>
-    <row r="380" spans="1:4">
+    <row r="380" spans="1:5">
       <c r="A380" s="62" t="s">
         <v>125</v>
       </c>
@@ -11292,7 +11293,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="381" spans="1:4">
+    <row r="381" spans="1:5">
       <c r="A381" s="62" t="s">
         <v>125</v>
       </c>
@@ -11306,7 +11307,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="382" spans="1:4">
+    <row r="382" spans="1:5">
       <c r="A382" s="62" t="s">
         <v>125</v>
       </c>
@@ -11320,7 +11321,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="383" spans="1:4">
+    <row r="383" spans="1:5">
       <c r="A383" s="62" t="s">
         <v>125</v>
       </c>
@@ -11334,7 +11335,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="384" spans="1:4">
+    <row r="384" spans="1:5">
       <c r="A384" s="62" t="s">
         <v>125</v>
       </c>
@@ -11344,7 +11345,7 @@
       <c r="C384" s="69" t="s">
         <v>1077</v>
       </c>
-      <c r="D384" s="65" t="s">
+      <c r="E384" s="65" t="s">
         <v>932</v>
       </c>
     </row>
@@ -11560,7 +11561,7 @@
       </c>
       <c r="D400" s="65"/>
     </row>
-    <row r="401" spans="1:4">
+    <row r="401" spans="1:5">
       <c r="A401" s="62" t="s">
         <v>125</v>
       </c>
@@ -11574,7 +11575,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="402" spans="1:4">
+    <row r="402" spans="1:5">
       <c r="A402" s="62" t="s">
         <v>125</v>
       </c>
@@ -11588,7 +11589,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="403" spans="1:4">
+    <row r="403" spans="1:5">
       <c r="A403" s="62" t="s">
         <v>125</v>
       </c>
@@ -11602,7 +11603,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="404" spans="1:4">
+    <row r="404" spans="1:5">
       <c r="A404" s="62" t="s">
         <v>125</v>
       </c>
@@ -11616,7 +11617,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="405" spans="1:4">
+    <row r="405" spans="1:5">
       <c r="A405" s="62" t="s">
         <v>125</v>
       </c>
@@ -11630,7 +11631,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="406" spans="1:4" ht="31.5">
+    <row r="406" spans="1:5" ht="31.5">
       <c r="A406" s="62" t="s">
         <v>125</v>
       </c>
@@ -11644,7 +11645,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="407" spans="1:4">
+    <row r="407" spans="1:5">
       <c r="A407" s="62" t="s">
         <v>125</v>
       </c>
@@ -11656,7 +11657,7 @@
       </c>
       <c r="D407" s="65"/>
     </row>
-    <row r="408" spans="1:4" ht="47.25">
+    <row r="408" spans="1:5" ht="47.25">
       <c r="A408" s="62" t="s">
         <v>125</v>
       </c>
@@ -11670,7 +11671,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="409" spans="1:4" ht="31.5">
+    <row r="409" spans="1:5" ht="31.5">
       <c r="A409" s="62" t="s">
         <v>125</v>
       </c>
@@ -11684,7 +11685,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="410" spans="1:4">
+    <row r="410" spans="1:5">
       <c r="A410" s="62" t="s">
         <v>125</v>
       </c>
@@ -11698,7 +11699,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="411" spans="1:4">
+    <row r="411" spans="1:5">
       <c r="A411" s="62" t="s">
         <v>125</v>
       </c>
@@ -11712,7 +11713,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="412" spans="1:4">
+    <row r="412" spans="1:5">
       <c r="A412" s="62" t="s">
         <v>125</v>
       </c>
@@ -11724,7 +11725,7 @@
       </c>
       <c r="D412" s="65"/>
     </row>
-    <row r="413" spans="1:4">
+    <row r="413" spans="1:5">
       <c r="A413" s="62" t="s">
         <v>125</v>
       </c>
@@ -11738,7 +11739,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="414" spans="1:4">
+    <row r="414" spans="1:5">
       <c r="A414" s="62" t="s">
         <v>125</v>
       </c>
@@ -11748,11 +11749,11 @@
       <c r="C414" s="69" t="s">
         <v>1066</v>
       </c>
-      <c r="D414" s="65" t="s">
+      <c r="E414" s="65" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="415" spans="1:4">
+    <row r="415" spans="1:5">
       <c r="A415" s="62" t="s">
         <v>125</v>
       </c>
@@ -11764,7 +11765,7 @@
       </c>
       <c r="D415" s="65"/>
     </row>
-    <row r="416" spans="1:4">
+    <row r="416" spans="1:5">
       <c r="A416" s="62" t="s">
         <v>125</v>
       </c>
@@ -11778,7 +11779,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="417" spans="1:4">
+    <row r="417" spans="1:5">
       <c r="A417" s="62" t="s">
         <v>125</v>
       </c>
@@ -11792,7 +11793,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="418" spans="1:4">
+    <row r="418" spans="1:5">
       <c r="A418" s="62" t="s">
         <v>125</v>
       </c>
@@ -11806,7 +11807,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="419" spans="1:4">
+    <row r="419" spans="1:5">
       <c r="A419" s="62" t="s">
         <v>125</v>
       </c>
@@ -11820,7 +11821,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="420" spans="1:4">
+    <row r="420" spans="1:5">
       <c r="A420" s="62" t="s">
         <v>125</v>
       </c>
@@ -11830,11 +11831,11 @@
       <c r="C420" s="69" t="s">
         <v>1077</v>
       </c>
-      <c r="D420" s="65" t="s">
+      <c r="E420" s="65" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="421" spans="1:4">
+    <row r="421" spans="1:5">
       <c r="A421" s="62" t="s">
         <v>125</v>
       </c>
@@ -11846,7 +11847,7 @@
       </c>
       <c r="D421" s="65"/>
     </row>
-    <row r="422" spans="1:4">
+    <row r="422" spans="1:5">
       <c r="A422" s="62" t="s">
         <v>125</v>
       </c>
@@ -11856,11 +11857,11 @@
       <c r="C422" s="72" t="s">
         <v>112</v>
       </c>
-      <c r="D422" s="65" t="s">
+      <c r="E422" s="65" t="s">
         <v>947</v>
       </c>
     </row>
-    <row r="423" spans="1:4">
+    <row r="423" spans="1:5">
       <c r="A423" s="62" t="s">
         <v>125</v>
       </c>
@@ -11870,11 +11871,11 @@
       <c r="C423" s="72" t="s">
         <v>94</v>
       </c>
-      <c r="D423" s="65" t="s">
+      <c r="E423" s="65" t="s">
         <v>947</v>
       </c>
     </row>
-    <row r="424" spans="1:4">
+    <row r="424" spans="1:5">
       <c r="A424" s="62" t="s">
         <v>125</v>
       </c>
@@ -11884,11 +11885,11 @@
       <c r="C424" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="D424" s="65" t="s">
+      <c r="E424" s="65" t="s">
         <v>947</v>
       </c>
     </row>
-    <row r="425" spans="1:4">
+    <row r="425" spans="1:5">
       <c r="A425" s="62" t="s">
         <v>125</v>
       </c>
@@ -11898,9 +11899,9 @@
       <c r="C425" s="64" t="s">
         <v>116</v>
       </c>
-      <c r="D425" s="65"/>
-    </row>
-    <row r="426" spans="1:4">
+      <c r="E425" s="65"/>
+    </row>
+    <row r="426" spans="1:5">
       <c r="A426" s="62" t="s">
         <v>125</v>
       </c>
@@ -11910,11 +11911,11 @@
       <c r="C426" s="72" t="s">
         <v>118</v>
       </c>
-      <c r="D426" s="65" t="s">
+      <c r="E426" s="65" t="s">
         <v>947</v>
       </c>
     </row>
-    <row r="427" spans="1:4">
+    <row r="427" spans="1:5">
       <c r="A427" s="62" t="s">
         <v>125</v>
       </c>
@@ -11924,11 +11925,11 @@
       <c r="C427" s="72" t="s">
         <v>94</v>
       </c>
-      <c r="D427" s="65" t="s">
+      <c r="E427" s="65" t="s">
         <v>947</v>
       </c>
     </row>
-    <row r="428" spans="1:4">
+    <row r="428" spans="1:5">
       <c r="A428" s="62" t="s">
         <v>125</v>
       </c>
@@ -11940,7 +11941,7 @@
       </c>
       <c r="D428" s="65"/>
     </row>
-    <row r="429" spans="1:4">
+    <row r="429" spans="1:5">
       <c r="A429" s="62" t="s">
         <v>125</v>
       </c>
@@ -11952,7 +11953,7 @@
       </c>
       <c r="D429" s="65"/>
     </row>
-    <row r="430" spans="1:4" ht="47.25">
+    <row r="430" spans="1:5" ht="47.25">
       <c r="A430" s="62" t="s">
         <v>125</v>
       </c>
@@ -11966,7 +11967,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="431" spans="1:4">
+    <row r="431" spans="1:5">
       <c r="A431" s="62" t="s">
         <v>125</v>
       </c>
@@ -11980,7 +11981,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="432" spans="1:4">
+    <row r="432" spans="1:5">
       <c r="A432" s="62" t="s">
         <v>125</v>
       </c>
@@ -11994,7 +11995,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="433" spans="1:4">
+    <row r="433" spans="1:5">
       <c r="A433" s="62" t="s">
         <v>125</v>
       </c>
@@ -12006,7 +12007,7 @@
       </c>
       <c r="D433" s="65"/>
     </row>
-    <row r="434" spans="1:4">
+    <row r="434" spans="1:5">
       <c r="A434" s="62" t="s">
         <v>125</v>
       </c>
@@ -12018,7 +12019,7 @@
       </c>
       <c r="D434" s="65"/>
     </row>
-    <row r="435" spans="1:4">
+    <row r="435" spans="1:5">
       <c r="A435" s="62" t="s">
         <v>125</v>
       </c>
@@ -12032,7 +12033,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="436" spans="1:4">
+    <row r="436" spans="1:5">
       <c r="A436" s="62" t="s">
         <v>125</v>
       </c>
@@ -12046,7 +12047,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="437" spans="1:4">
+    <row r="437" spans="1:5">
       <c r="A437" s="62" t="s">
         <v>125</v>
       </c>
@@ -12056,11 +12057,11 @@
       <c r="C437" s="69" t="s">
         <v>1170</v>
       </c>
-      <c r="D437" s="65" t="s">
+      <c r="E437" s="65" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="438" spans="1:4">
+    <row r="438" spans="1:5">
       <c r="A438" s="62" t="s">
         <v>125</v>
       </c>
@@ -12074,7 +12075,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="439" spans="1:4" ht="31.5">
+    <row r="439" spans="1:5" ht="31.5">
       <c r="A439" s="62" t="s">
         <v>125</v>
       </c>
@@ -12088,7 +12089,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="440" spans="1:4">
+    <row r="440" spans="1:5">
       <c r="A440" s="62" t="s">
         <v>125</v>
       </c>
@@ -12102,7 +12103,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="441" spans="1:4">
+    <row r="441" spans="1:5">
       <c r="A441" s="62" t="s">
         <v>125</v>
       </c>
@@ -12114,7 +12115,7 @@
       </c>
       <c r="D441" s="65"/>
     </row>
-    <row r="442" spans="1:4">
+    <row r="442" spans="1:5">
       <c r="A442" s="62" t="s">
         <v>125</v>
       </c>
@@ -12128,7 +12129,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="443" spans="1:4">
+    <row r="443" spans="1:5">
       <c r="A443" s="62" t="s">
         <v>125</v>
       </c>
@@ -12138,11 +12139,11 @@
       <c r="C443" s="69" t="s">
         <v>1066</v>
       </c>
-      <c r="D443" s="65" t="s">
+      <c r="E443" s="65" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="444" spans="1:4">
+    <row r="444" spans="1:5">
       <c r="A444" s="62" t="s">
         <v>125</v>
       </c>
@@ -12154,7 +12155,7 @@
       </c>
       <c r="D444" s="65"/>
     </row>
-    <row r="445" spans="1:4">
+    <row r="445" spans="1:5">
       <c r="A445" s="62" t="s">
         <v>125</v>
       </c>
@@ -12168,7 +12169,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="446" spans="1:4">
+    <row r="446" spans="1:5">
       <c r="A446" s="62" t="s">
         <v>125</v>
       </c>
@@ -12182,7 +12183,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="447" spans="1:4">
+    <row r="447" spans="1:5">
       <c r="A447" s="62" t="s">
         <v>125</v>
       </c>
@@ -12196,7 +12197,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="448" spans="1:4">
+    <row r="448" spans="1:5">
       <c r="A448" s="62" t="s">
         <v>125</v>
       </c>
@@ -12210,7 +12211,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="449" spans="1:4">
+    <row r="449" spans="1:5">
       <c r="A449" s="62" t="s">
         <v>125</v>
       </c>
@@ -12220,7 +12221,7 @@
       <c r="C449" s="69" t="s">
         <v>1077</v>
       </c>
-      <c r="D449" s="65" t="s">
+      <c r="E449" s="65" t="s">
         <v>932</v>
       </c>
     </row>
@@ -14619,7 +14620,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>

</xml_diff>

<commit_message>
Temporarily removed 73-4.37 from sheet
</commit_message>
<xml_diff>
--- a/docs/coverage-testing/85b_test_definitions_PIV_ICAM_Test_Cards_Exploded.xlsx
+++ b/docs/coverage-testing/85b_test_definitions_PIV_ICAM_Test_Cards_Exploded.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\docs\coverage-testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6D747B-3B42-4492-902B-8CAA28ACECBF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D21658B-2B8D-4CB8-9453-1494D48B34CE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="525" windowWidth="25680" windowHeight="16305" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6085,8 +6085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{539C8DD9-7E09-4AC9-B53E-1B766442D166}">
   <dimension ref="A1:E449"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A276" workbookViewId="0">
-      <selection activeCell="C282" sqref="C282"/>
+    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
+      <selection activeCell="E282" sqref="E282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -9832,7 +9832,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="273" spans="1:4" ht="31.5">
+    <row r="273" spans="1:5" ht="31.5">
       <c r="A273" s="62" t="s">
         <v>125</v>
       </c>
@@ -9846,7 +9846,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="274" spans="1:4" ht="31.5">
+    <row r="274" spans="1:5" ht="31.5">
       <c r="A274" s="62" t="s">
         <v>125</v>
       </c>
@@ -9860,7 +9860,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="275" spans="1:4" ht="31.5">
+    <row r="275" spans="1:5" ht="31.5">
       <c r="A275" s="62" t="s">
         <v>125</v>
       </c>
@@ -9874,7 +9874,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="276" spans="1:4" ht="47.25">
+    <row r="276" spans="1:5" ht="47.25">
       <c r="A276" s="62" t="s">
         <v>125</v>
       </c>
@@ -9888,7 +9888,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="277" spans="1:4" ht="47.25">
+    <row r="277" spans="1:5" ht="47.25">
       <c r="A277" s="62" t="s">
         <v>125</v>
       </c>
@@ -9902,7 +9902,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="278" spans="1:4" ht="47.25">
+    <row r="278" spans="1:5" ht="47.25">
       <c r="A278" s="62" t="s">
         <v>125</v>
       </c>
@@ -9916,7 +9916,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="279" spans="1:4" ht="31.5">
+    <row r="279" spans="1:5" ht="31.5">
       <c r="A279" s="62" t="s">
         <v>125</v>
       </c>
@@ -9930,7 +9930,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="280" spans="1:4">
+    <row r="280" spans="1:5">
       <c r="A280" s="62" t="s">
         <v>125</v>
       </c>
@@ -9942,7 +9942,7 @@
       </c>
       <c r="D280" s="65"/>
     </row>
-    <row r="281" spans="1:4">
+    <row r="281" spans="1:5">
       <c r="A281" s="62" t="s">
         <v>125</v>
       </c>
@@ -9954,7 +9954,7 @@
       </c>
       <c r="D281" s="65"/>
     </row>
-    <row r="282" spans="1:4" ht="31.5">
+    <row r="282" spans="1:5" ht="31.5">
       <c r="A282" s="62" t="s">
         <v>125</v>
       </c>
@@ -9964,11 +9964,11 @@
       <c r="C282" s="72" t="s">
         <v>438</v>
       </c>
-      <c r="D282" s="65" t="s">
+      <c r="E282" s="73" t="s">
         <v>1019</v>
       </c>
     </row>
-    <row r="283" spans="1:4">
+    <row r="283" spans="1:5">
       <c r="A283" s="62" t="s">
         <v>125</v>
       </c>
@@ -9980,7 +9980,7 @@
       </c>
       <c r="D283" s="65"/>
     </row>
-    <row r="284" spans="1:4" ht="31.5">
+    <row r="284" spans="1:5" ht="31.5">
       <c r="A284" s="62" t="s">
         <v>125</v>
       </c>
@@ -9994,7 +9994,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="285" spans="1:4">
+    <row r="285" spans="1:5">
       <c r="A285" s="62" t="s">
         <v>125</v>
       </c>
@@ -10008,7 +10008,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="286" spans="1:4">
+    <row r="286" spans="1:5">
       <c r="A286" s="62" t="s">
         <v>125</v>
       </c>
@@ -10022,7 +10022,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="287" spans="1:4" ht="31.5">
+    <row r="287" spans="1:5" ht="31.5">
       <c r="A287" s="62" t="s">
         <v>125</v>
       </c>
@@ -10036,7 +10036,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="288" spans="1:4">
+    <row r="288" spans="1:5">
       <c r="A288" s="62" t="s">
         <v>125</v>
       </c>
@@ -12230,6 +12230,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -12419,7 +12420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C19" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C7" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Removed more unicode characters
</commit_message>
<xml_diff>
--- a/docs/coverage-testing/85b_test_definitions_PIV_ICAM_Test_Cards_Exploded.xlsx
+++ b/docs/coverage-testing/85b_test_definitions_PIV_ICAM_Test_Cards_Exploded.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\docs\coverage-testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1736F77D-EFF4-43AA-8CD5-6E10433BAEEB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA7F038-5C16-4313-9ECD-987754A077C5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4125" yWindow="240" windowWidth="25680" windowHeight="16305" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2776" uniqueCount="1187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2776" uniqueCount="1186">
   <si>
     <t>Test Case</t>
   </si>
@@ -3073,9 +3073,6 @@
   </si>
   <si>
     <t>Certificates field in the SignedData contains a single certificate that can be used to verify the digital signature in the SignerInfo. If the certificates field is omitted, then the certificates field of the SignedData for the CHUID contains the certificate that can be used to verify the digital signature.</t>
-  </si>
-  <si>
-    <t>signedAttrs of the SignerInfo includes the entryUUID (OID = 1.3.6.1.1.16.4) attribute and that it is the same value as the Card UUID in the GUID data element of the PIV card’s CHUID data object.</t>
   </si>
   <si>
     <t>10.3</t>
@@ -6088,8 +6085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{539C8DD9-7E09-4AC9-B53E-1B766442D166}">
   <dimension ref="A1:E449"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
-      <selection activeCell="C247" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A385" workbookViewId="0">
+      <selection activeCell="C308" sqref="C308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -9679,7 +9676,7 @@
         <v>421</v>
       </c>
       <c r="C261" s="72" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="D261" s="65" t="s">
         <v>423</v>
@@ -9690,7 +9687,7 @@
         <v>125</v>
       </c>
       <c r="B262" s="63" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="C262" s="64" t="s">
         <v>80</v>
@@ -9702,7 +9699,7 @@
         <v>125</v>
       </c>
       <c r="B263" s="63" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="C263" s="72" t="s">
         <v>78</v>
@@ -9742,7 +9739,7 @@
         <v>125</v>
       </c>
       <c r="B266" s="63" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="C266" s="72" t="s">
         <v>406</v>
@@ -9826,7 +9823,7 @@
         <v>125</v>
       </c>
       <c r="B272" s="63" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="C272" s="72" t="s">
         <v>1001</v>
@@ -9840,7 +9837,7 @@
         <v>125</v>
       </c>
       <c r="B273" s="63" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="C273" s="72" t="s">
         <v>1003</v>
@@ -9910,7 +9907,7 @@
         <v>125</v>
       </c>
       <c r="B278" s="63" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="C278" s="72" t="s">
         <v>1009</v>
@@ -9927,7 +9924,7 @@
         <v>436</v>
       </c>
       <c r="C279" s="72" t="s">
-        <v>1010</v>
+        <v>1185</v>
       </c>
       <c r="D279" s="65" t="s">
         <v>423</v>
@@ -9938,7 +9935,7 @@
         <v>125</v>
       </c>
       <c r="B280" s="63" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="C280" s="64" t="s">
         <v>23</v>
@@ -9950,7 +9947,7 @@
         <v>125</v>
       </c>
       <c r="B281" s="63" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="C281" s="70" t="s">
         <v>84</v>
@@ -9968,7 +9965,7 @@
         <v>438</v>
       </c>
       <c r="E282" s="73" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="283" spans="1:5">
@@ -9976,7 +9973,7 @@
         <v>125</v>
       </c>
       <c r="B283" s="63" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="C283" s="72" t="s">
         <v>78</v>
@@ -10086,7 +10083,7 @@
         <v>125</v>
       </c>
       <c r="B291" s="63" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="C291" s="74" t="s">
         <v>87</v>
@@ -10098,7 +10095,7 @@
         <v>125</v>
       </c>
       <c r="B292" s="63" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="C292" s="75" t="s">
         <v>78</v>
@@ -10110,7 +10107,7 @@
         <v>125</v>
       </c>
       <c r="B293" s="63" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="C293" s="62" t="s">
         <v>997</v>
@@ -10124,7 +10121,7 @@
         <v>125</v>
       </c>
       <c r="B294" s="63" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="C294" s="62" t="s">
         <v>405</v>
@@ -10138,7 +10135,7 @@
         <v>125</v>
       </c>
       <c r="B295" s="63" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="C295" s="62" t="s">
         <v>406</v>
@@ -10152,7 +10149,7 @@
         <v>125</v>
       </c>
       <c r="B296" s="63" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="C296" s="62" t="s">
         <v>999</v>
@@ -10166,7 +10163,7 @@
         <v>125</v>
       </c>
       <c r="B297" s="63" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="C297" s="62" t="s">
         <v>378</v>
@@ -10180,7 +10177,7 @@
         <v>125</v>
       </c>
       <c r="B298" s="63" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="C298" s="62" t="s">
         <v>381</v>
@@ -10194,7 +10191,7 @@
         <v>125</v>
       </c>
       <c r="B299" s="63" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="C299" s="62" t="s">
         <v>411</v>
@@ -10208,7 +10205,7 @@
         <v>125</v>
       </c>
       <c r="B300" s="63" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="C300" s="62" t="s">
         <v>892</v>
@@ -10222,7 +10219,7 @@
         <v>125</v>
       </c>
       <c r="B301" s="63" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="C301" s="62" t="s">
         <v>1001</v>
@@ -10236,7 +10233,7 @@
         <v>125</v>
       </c>
       <c r="B302" s="63" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="C302" s="62" t="s">
         <v>1003</v>
@@ -10250,7 +10247,7 @@
         <v>125</v>
       </c>
       <c r="B303" s="63" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="C303" s="62" t="s">
         <v>416</v>
@@ -10264,7 +10261,7 @@
         <v>125</v>
       </c>
       <c r="B304" s="63" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="C304" s="62" t="s">
         <v>1004</v>
@@ -10278,7 +10275,7 @@
         <v>125</v>
       </c>
       <c r="B305" s="63" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="C305" s="62" t="s">
         <v>1005</v>
@@ -10292,7 +10289,7 @@
         <v>125</v>
       </c>
       <c r="B306" s="63" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="C306" s="62" t="s">
         <v>1007</v>
@@ -10306,7 +10303,7 @@
         <v>125</v>
       </c>
       <c r="B307" s="63" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="C307" s="62" t="s">
         <v>1009</v>
@@ -10320,10 +10317,10 @@
         <v>125</v>
       </c>
       <c r="B308" s="63" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C308" s="62" t="s">
-        <v>1010</v>
+        <v>1185</v>
       </c>
       <c r="D308" s="65" t="s">
         <v>423</v>
@@ -10334,7 +10331,7 @@
         <v>125</v>
       </c>
       <c r="B309" s="59" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="C309" s="76" t="s">
         <v>90</v>
@@ -10346,7 +10343,7 @@
         <v>125</v>
       </c>
       <c r="B310" s="63" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="C310" s="74" t="s">
         <v>92</v>
@@ -10358,7 +10355,7 @@
         <v>125</v>
       </c>
       <c r="B311" s="63" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="C311" s="75" t="s">
         <v>94</v>
@@ -10370,10 +10367,10 @@
         <v>125</v>
       </c>
       <c r="B312" s="63" t="s">
+        <v>1041</v>
+      </c>
+      <c r="C312" s="72" t="s">
         <v>1042</v>
-      </c>
-      <c r="C312" s="72" t="s">
-        <v>1043</v>
       </c>
       <c r="D312" s="65" t="s">
         <v>414</v>
@@ -10401,7 +10398,7 @@
         <v>463</v>
       </c>
       <c r="C314" s="72" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D314" s="65" t="s">
         <v>402</v>
@@ -10412,7 +10409,7 @@
         <v>125</v>
       </c>
       <c r="B315" s="63" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="C315" s="70" t="s">
         <v>96</v>
@@ -10424,10 +10421,10 @@
         <v>125</v>
       </c>
       <c r="B316" s="63" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C316" s="72" t="s">
         <v>1046</v>
-      </c>
-      <c r="C316" s="72" t="s">
-        <v>1047</v>
       </c>
       <c r="D316" s="65" t="s">
         <v>465</v>
@@ -10438,10 +10435,10 @@
         <v>125</v>
       </c>
       <c r="B317" s="63" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C317" s="72" t="s">
         <v>1048</v>
-      </c>
-      <c r="C317" s="72" t="s">
-        <v>1049</v>
       </c>
       <c r="D317" s="65" t="s">
         <v>467</v>
@@ -10452,10 +10449,10 @@
         <v>125</v>
       </c>
       <c r="B318" s="63" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C318" s="62" t="s">
         <v>1050</v>
-      </c>
-      <c r="C318" s="62" t="s">
-        <v>1051</v>
       </c>
       <c r="D318" s="65" t="s">
         <v>469</v>
@@ -10466,10 +10463,10 @@
         <v>125</v>
       </c>
       <c r="B319" s="63" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C319" s="72" t="s">
         <v>1052</v>
-      </c>
-      <c r="C319" s="72" t="s">
-        <v>1053</v>
       </c>
       <c r="D319" s="65" t="s">
         <v>471</v>
@@ -10480,10 +10477,10 @@
         <v>125</v>
       </c>
       <c r="B320" s="63" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C320" s="70" t="s">
         <v>1054</v>
-      </c>
-      <c r="C320" s="70" t="s">
-        <v>1055</v>
       </c>
       <c r="D320" s="65"/>
     </row>
@@ -10537,7 +10534,7 @@
         <v>480</v>
       </c>
       <c r="C324" s="72" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="D324" s="65" t="s">
         <v>482</v>
@@ -10562,10 +10559,10 @@
         <v>125</v>
       </c>
       <c r="B326" s="63" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C326" s="70" t="s">
         <v>1057</v>
-      </c>
-      <c r="C326" s="70" t="s">
-        <v>1058</v>
       </c>
       <c r="D326" s="65" t="s">
         <v>488</v>
@@ -10621,7 +10618,7 @@
         <v>493</v>
       </c>
       <c r="C330" s="72" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="D330" s="65" t="s">
         <v>495</v>
@@ -10635,7 +10632,7 @@
         <v>496</v>
       </c>
       <c r="C331" s="72" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D331" s="65" t="s">
         <v>498</v>
@@ -10646,10 +10643,10 @@
         <v>125</v>
       </c>
       <c r="B332" s="63" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C332" s="70" t="s">
         <v>1061</v>
-      </c>
-      <c r="C332" s="70" t="s">
-        <v>1062</v>
       </c>
       <c r="D332" s="65"/>
     </row>
@@ -10658,10 +10655,10 @@
         <v>125</v>
       </c>
       <c r="B333" s="63" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C333" s="72" t="s">
         <v>1063</v>
-      </c>
-      <c r="C333" s="72" t="s">
-        <v>1064</v>
       </c>
       <c r="D333" s="65" t="s">
         <v>479</v>
@@ -10672,10 +10669,10 @@
         <v>125</v>
       </c>
       <c r="B334" s="63" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C334" s="69" t="s">
         <v>1065</v>
-      </c>
-      <c r="C334" s="69" t="s">
-        <v>1066</v>
       </c>
       <c r="E334" s="65" t="s">
         <v>932</v>
@@ -10686,10 +10683,10 @@
         <v>125</v>
       </c>
       <c r="B335" s="63" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C335" s="70" t="s">
         <v>1067</v>
-      </c>
-      <c r="C335" s="70" t="s">
-        <v>1068</v>
       </c>
       <c r="D335" s="65"/>
     </row>
@@ -10698,7 +10695,7 @@
         <v>125</v>
       </c>
       <c r="B336" s="63" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="C336" s="72" t="s">
         <v>473</v>
@@ -10712,10 +10709,10 @@
         <v>125</v>
       </c>
       <c r="B337" s="63" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C337" s="72" t="s">
         <v>1070</v>
-      </c>
-      <c r="C337" s="72" t="s">
-        <v>1071</v>
       </c>
       <c r="D337" s="73" t="s">
         <v>477</v>
@@ -10726,10 +10723,10 @@
         <v>125</v>
       </c>
       <c r="B338" s="63" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C338" s="72" t="s">
         <v>1072</v>
-      </c>
-      <c r="C338" s="72" t="s">
-        <v>1073</v>
       </c>
       <c r="D338" s="65" t="s">
         <v>479</v>
@@ -10740,10 +10737,10 @@
         <v>125</v>
       </c>
       <c r="B339" s="63" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C339" s="72" t="s">
         <v>1074</v>
-      </c>
-      <c r="C339" s="72" t="s">
-        <v>1075</v>
       </c>
       <c r="D339" s="65" t="s">
         <v>479</v>
@@ -10754,10 +10751,10 @@
         <v>125</v>
       </c>
       <c r="B340" s="63" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C340" s="69" t="s">
         <v>1076</v>
-      </c>
-      <c r="C340" s="69" t="s">
-        <v>1077</v>
       </c>
       <c r="E340" s="65" t="s">
         <v>932</v>
@@ -10768,7 +10765,7 @@
         <v>125</v>
       </c>
       <c r="B341" s="63" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="C341" s="64" t="s">
         <v>98</v>
@@ -10780,7 +10777,7 @@
         <v>125</v>
       </c>
       <c r="B342" s="63" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="C342" s="72" t="s">
         <v>94</v>
@@ -10795,7 +10792,7 @@
         <v>499</v>
       </c>
       <c r="C343" s="72" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="D343" s="65" t="s">
         <v>414</v>
@@ -10809,7 +10806,7 @@
         <v>500</v>
       </c>
       <c r="C344" s="72" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="D344" s="65" t="s">
         <v>402</v>
@@ -10820,10 +10817,10 @@
         <v>125</v>
       </c>
       <c r="B345" s="63" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="C345" s="72" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D345" s="77" t="s">
         <v>402</v>
@@ -10834,7 +10831,7 @@
         <v>125</v>
       </c>
       <c r="B346" s="63" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="C346" s="70" t="s">
         <v>96</v>
@@ -10846,10 +10843,10 @@
         <v>125</v>
       </c>
       <c r="B347" s="63" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C347" s="70" t="s">
         <v>1083</v>
-      </c>
-      <c r="C347" s="70" t="s">
-        <v>1084</v>
       </c>
       <c r="D347" s="65"/>
     </row>
@@ -10861,7 +10858,7 @@
         <v>502</v>
       </c>
       <c r="C348" s="62" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="D348" s="65" t="s">
         <v>501</v>
@@ -10889,7 +10886,7 @@
         <v>507</v>
       </c>
       <c r="C350" s="72" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="D350" s="65" t="s">
         <v>485</v>
@@ -10903,7 +10900,7 @@
         <v>508</v>
       </c>
       <c r="C351" s="72" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="D351" s="65" t="s">
         <v>495</v>
@@ -10917,7 +10914,7 @@
         <v>509</v>
       </c>
       <c r="C352" s="72" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="D352" s="65" t="s">
         <v>498</v>
@@ -10928,10 +10925,10 @@
         <v>125</v>
       </c>
       <c r="B353" s="63" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C353" s="72" t="s">
         <v>1089</v>
-      </c>
-      <c r="C353" s="72" t="s">
-        <v>1090</v>
       </c>
       <c r="D353" s="65" t="s">
         <v>471</v>
@@ -10942,10 +10939,10 @@
         <v>125</v>
       </c>
       <c r="B354" s="63" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="C354" s="70" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="D354" s="65"/>
     </row>
@@ -10954,10 +10951,10 @@
         <v>125</v>
       </c>
       <c r="B355" s="63" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C355" s="72" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="D355" s="65" t="s">
         <v>479</v>
@@ -10968,10 +10965,10 @@
         <v>125</v>
       </c>
       <c r="B356" s="63" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="C356" s="69" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="E356" s="65" t="s">
         <v>932</v>
@@ -10982,10 +10979,10 @@
         <v>125</v>
       </c>
       <c r="B357" s="63" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="C357" s="70" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="D357" s="65"/>
     </row>
@@ -10994,7 +10991,7 @@
         <v>125</v>
       </c>
       <c r="B358" s="63" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="C358" s="72" t="s">
         <v>473</v>
@@ -11008,10 +11005,10 @@
         <v>125</v>
       </c>
       <c r="B359" s="63" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C359" s="72" t="s">
         <v>1096</v>
-      </c>
-      <c r="C359" s="72" t="s">
-        <v>1097</v>
       </c>
       <c r="D359" s="73" t="s">
         <v>477</v>
@@ -11022,10 +11019,10 @@
         <v>125</v>
       </c>
       <c r="B360" s="63" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="C360" s="72" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="D360" s="65" t="s">
         <v>479</v>
@@ -11036,10 +11033,10 @@
         <v>125</v>
       </c>
       <c r="B361" s="63" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="C361" s="72" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="D361" s="65" t="s">
         <v>479</v>
@@ -11050,10 +11047,10 @@
         <v>125</v>
       </c>
       <c r="B362" s="63" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="C362" s="69" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="E362" s="65" t="s">
         <v>932</v>
@@ -11064,7 +11061,7 @@
         <v>125</v>
       </c>
       <c r="B363" s="63" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="C363" s="64" t="s">
         <v>102</v>
@@ -11076,7 +11073,7 @@
         <v>125</v>
       </c>
       <c r="B364" s="63" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="C364" s="70" t="s">
         <v>94</v>
@@ -11105,7 +11102,7 @@
         <v>511</v>
       </c>
       <c r="C366" s="62" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="D366" s="65" t="s">
         <v>402</v>
@@ -11116,7 +11113,7 @@
         <v>125</v>
       </c>
       <c r="B367" s="63" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="C367" s="72" t="s">
         <v>460</v>
@@ -11130,7 +11127,7 @@
         <v>125</v>
       </c>
       <c r="B368" s="63" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="C368" s="70" t="s">
         <v>96</v>
@@ -11142,10 +11139,10 @@
         <v>125</v>
       </c>
       <c r="B369" s="63" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="C369" s="70" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="D369" s="65"/>
     </row>
@@ -11157,7 +11154,7 @@
         <v>512</v>
       </c>
       <c r="C370" s="72" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="D370" s="65" t="s">
         <v>513</v>
@@ -11171,7 +11168,7 @@
         <v>514</v>
       </c>
       <c r="C371" s="72" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D371" s="65" t="s">
         <v>506</v>
@@ -11185,7 +11182,7 @@
         <v>515</v>
       </c>
       <c r="C372" s="72" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="D372" s="65" t="s">
         <v>467</v>
@@ -11199,7 +11196,7 @@
         <v>516</v>
       </c>
       <c r="C373" s="72" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D373" s="65" t="s">
         <v>485</v>
@@ -11213,7 +11210,7 @@
         <v>517</v>
       </c>
       <c r="C374" s="72" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="D374" s="65" t="s">
         <v>498</v>
@@ -11224,10 +11221,10 @@
         <v>125</v>
       </c>
       <c r="B375" s="63" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="C375" s="72" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="D375" s="65" t="s">
         <v>471</v>
@@ -11238,10 +11235,10 @@
         <v>125</v>
       </c>
       <c r="B376" s="63" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="C376" s="70" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="D376" s="65"/>
     </row>
@@ -11250,10 +11247,10 @@
         <v>125</v>
       </c>
       <c r="B377" s="63" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C377" s="72" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="D377" s="65" t="s">
         <v>479</v>
@@ -11264,10 +11261,10 @@
         <v>125</v>
       </c>
       <c r="B378" s="63" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="C378" s="69" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="E378" s="65" t="s">
         <v>932</v>
@@ -11278,10 +11275,10 @@
         <v>125</v>
       </c>
       <c r="B379" s="63" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="C379" s="70" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="D379" s="65"/>
     </row>
@@ -11290,7 +11287,7 @@
         <v>125</v>
       </c>
       <c r="B380" s="63" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="C380" s="72" t="s">
         <v>473</v>
@@ -11304,10 +11301,10 @@
         <v>125</v>
       </c>
       <c r="B381" s="63" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="C381" s="72" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="D381" s="73" t="s">
         <v>477</v>
@@ -11318,10 +11315,10 @@
         <v>125</v>
       </c>
       <c r="B382" s="63" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C382" s="72" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="D382" s="65" t="s">
         <v>479</v>
@@ -11332,10 +11329,10 @@
         <v>125</v>
       </c>
       <c r="B383" s="63" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="C383" s="63" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="D383" s="65" t="s">
         <v>479</v>
@@ -11346,10 +11343,10 @@
         <v>125</v>
       </c>
       <c r="B384" s="63" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="C384" s="69" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="E384" s="65" t="s">
         <v>932</v>
@@ -11360,7 +11357,7 @@
         <v>125</v>
       </c>
       <c r="B385" s="63" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="C385" s="64" t="s">
         <v>106</v>
@@ -11372,7 +11369,7 @@
         <v>125</v>
       </c>
       <c r="B386" s="63" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="C386" s="70" t="s">
         <v>94</v>
@@ -11401,7 +11398,7 @@
         <v>519</v>
       </c>
       <c r="C388" s="72" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="D388" s="65" t="s">
         <v>402</v>
@@ -11412,7 +11409,7 @@
         <v>125</v>
       </c>
       <c r="B389" s="63" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C389" s="72" t="s">
         <v>460</v>
@@ -11426,7 +11423,7 @@
         <v>125</v>
       </c>
       <c r="B390" s="63" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="C390" s="70" t="s">
         <v>96</v>
@@ -11438,10 +11435,10 @@
         <v>125</v>
       </c>
       <c r="B391" s="63" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C391" s="70" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="D391" s="65"/>
     </row>
@@ -11453,7 +11450,7 @@
         <v>520</v>
       </c>
       <c r="C392" s="63" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="D392" s="65" t="s">
         <v>501</v>
@@ -11467,7 +11464,7 @@
         <v>521</v>
       </c>
       <c r="C393" s="72" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="D393" s="65" t="s">
         <v>465</v>
@@ -11481,7 +11478,7 @@
         <v>522</v>
       </c>
       <c r="C394" s="72" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D394" s="65" t="s">
         <v>467</v>
@@ -11495,7 +11492,7 @@
         <v>523</v>
       </c>
       <c r="C395" s="62" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="D395" s="65" t="s">
         <v>471</v>
@@ -11506,10 +11503,10 @@
         <v>125</v>
       </c>
       <c r="B396" s="63" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C396" s="70" t="s">
         <v>1131</v>
-      </c>
-      <c r="C396" s="70" t="s">
-        <v>1132</v>
       </c>
       <c r="D396" s="65"/>
     </row>
@@ -11521,7 +11518,7 @@
         <v>525</v>
       </c>
       <c r="C397" s="62" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="D397" s="65" t="s">
         <v>526</v>
@@ -11535,7 +11532,7 @@
         <v>527</v>
       </c>
       <c r="C398" s="62" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="D398" s="65" t="s">
         <v>528</v>
@@ -11546,10 +11543,10 @@
         <v>125</v>
       </c>
       <c r="B399" s="63" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C399" s="62" t="s">
         <v>1135</v>
-      </c>
-      <c r="C399" s="62" t="s">
-        <v>1136</v>
       </c>
       <c r="D399" s="73" t="s">
         <v>528</v>
@@ -11560,10 +11557,10 @@
         <v>125</v>
       </c>
       <c r="B400" s="63" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="C400" s="70" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="D400" s="65"/>
     </row>
@@ -11589,7 +11586,7 @@
         <v>530</v>
       </c>
       <c r="C402" s="72" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="D402" s="65" t="s">
         <v>477</v>
@@ -11603,7 +11600,7 @@
         <v>531</v>
       </c>
       <c r="C403" s="72" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="D403" s="65" t="s">
         <v>479</v>
@@ -11614,10 +11611,10 @@
         <v>125</v>
       </c>
       <c r="B404" s="63" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="C404" s="63" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="D404" s="63" t="s">
         <v>479</v>
@@ -11631,7 +11628,7 @@
         <v>532</v>
       </c>
       <c r="C405" s="72" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="D405" s="65" t="s">
         <v>482</v>
@@ -11645,7 +11642,7 @@
         <v>533</v>
       </c>
       <c r="C406" s="72" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D406" s="65" t="s">
         <v>485</v>
@@ -11656,10 +11653,10 @@
         <v>125</v>
       </c>
       <c r="B407" s="63" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="C407" s="70" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="D407" s="65"/>
     </row>
@@ -11668,7 +11665,7 @@
         <v>125</v>
       </c>
       <c r="B408" s="63" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="C408" s="72" t="s">
         <v>487</v>
@@ -11682,7 +11679,7 @@
         <v>125</v>
       </c>
       <c r="B409" s="63" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="C409" s="72" t="s">
         <v>490</v>
@@ -11696,10 +11693,10 @@
         <v>125</v>
       </c>
       <c r="B410" s="63" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C410" s="72" t="s">
         <v>1143</v>
-      </c>
-      <c r="C410" s="72" t="s">
-        <v>1144</v>
       </c>
       <c r="D410" s="65" t="s">
         <v>488</v>
@@ -11710,10 +11707,10 @@
         <v>125</v>
       </c>
       <c r="B411" s="63" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="C411" s="72" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="D411" s="65" t="s">
         <v>498</v>
@@ -11724,10 +11721,10 @@
         <v>125</v>
       </c>
       <c r="B412" s="63" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="C412" s="70" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="D412" s="65"/>
     </row>
@@ -11736,10 +11733,10 @@
         <v>125</v>
       </c>
       <c r="B413" s="63" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="C413" s="72" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="D413" s="65" t="s">
         <v>479</v>
@@ -11750,10 +11747,10 @@
         <v>125</v>
       </c>
       <c r="B414" s="63" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="C414" s="69" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="E414" s="65" t="s">
         <v>932</v>
@@ -11764,10 +11761,10 @@
         <v>125</v>
       </c>
       <c r="B415" s="63" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="C415" s="70" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="D415" s="65"/>
     </row>
@@ -11776,7 +11773,7 @@
         <v>125</v>
       </c>
       <c r="B416" s="63" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="C416" s="72" t="s">
         <v>473</v>
@@ -11790,10 +11787,10 @@
         <v>125</v>
       </c>
       <c r="B417" s="63" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="C417" s="72" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="D417" s="73" t="s">
         <v>477</v>
@@ -11804,10 +11801,10 @@
         <v>125</v>
       </c>
       <c r="B418" s="63" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="C418" s="72" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="D418" s="65" t="s">
         <v>479</v>
@@ -11818,10 +11815,10 @@
         <v>125</v>
       </c>
       <c r="B419" s="63" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="C419" s="63" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="D419" s="65" t="s">
         <v>479</v>
@@ -11832,10 +11829,10 @@
         <v>125</v>
       </c>
       <c r="B420" s="63" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="C420" s="69" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="E420" s="65" t="s">
         <v>932</v>
@@ -11858,7 +11855,7 @@
         <v>125</v>
       </c>
       <c r="B422" s="63" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="C422" s="72" t="s">
         <v>112</v>
@@ -11872,7 +11869,7 @@
         <v>125</v>
       </c>
       <c r="B423" s="63" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C423" s="72" t="s">
         <v>94</v>
@@ -11886,7 +11883,7 @@
         <v>125</v>
       </c>
       <c r="B424" s="63" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="C424" s="72" t="s">
         <v>96</v>
@@ -11912,7 +11909,7 @@
         <v>125</v>
       </c>
       <c r="B426" s="63" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="C426" s="72" t="s">
         <v>118</v>
@@ -11926,7 +11923,7 @@
         <v>125</v>
       </c>
       <c r="B427" s="63" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="C427" s="72" t="s">
         <v>94</v>
@@ -11952,7 +11949,7 @@
         <v>125</v>
       </c>
       <c r="B429" s="63" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="C429" s="70" t="s">
         <v>94</v>
@@ -11964,7 +11961,7 @@
         <v>125</v>
       </c>
       <c r="B430" s="63" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="C430" s="72" t="s">
         <v>459</v>
@@ -11978,10 +11975,10 @@
         <v>125</v>
       </c>
       <c r="B431" s="63" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="C431" s="72" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="D431" s="65" t="s">
         <v>402</v>
@@ -11992,7 +11989,7 @@
         <v>125</v>
       </c>
       <c r="B432" s="63" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="C432" s="72" t="s">
         <v>460</v>
@@ -12006,7 +12003,7 @@
         <v>125</v>
       </c>
       <c r="B433" s="63" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="C433" s="70" t="s">
         <v>96</v>
@@ -12018,10 +12015,10 @@
         <v>125</v>
       </c>
       <c r="B434" s="63" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="C434" s="70" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="D434" s="65"/>
     </row>
@@ -12030,10 +12027,10 @@
         <v>125</v>
       </c>
       <c r="B435" s="63" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C435" s="72" t="s">
         <v>1166</v>
-      </c>
-      <c r="C435" s="72" t="s">
-        <v>1167</v>
       </c>
       <c r="D435" s="65" t="s">
         <v>465</v>
@@ -12044,10 +12041,10 @@
         <v>125</v>
       </c>
       <c r="B436" s="63" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="C436" s="72" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D436" s="65" t="s">
         <v>467</v>
@@ -12058,10 +12055,10 @@
         <v>125</v>
       </c>
       <c r="B437" s="63" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C437" s="69" t="s">
         <v>1169</v>
-      </c>
-      <c r="C437" s="69" t="s">
-        <v>1170</v>
       </c>
       <c r="E437" s="65" t="s">
         <v>932</v>
@@ -12072,10 +12069,10 @@
         <v>125</v>
       </c>
       <c r="B438" s="63" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C438" s="62" t="s">
         <v>1171</v>
-      </c>
-      <c r="C438" s="62" t="s">
-        <v>1172</v>
       </c>
       <c r="D438" s="65" t="s">
         <v>498</v>
@@ -12086,10 +12083,10 @@
         <v>125</v>
       </c>
       <c r="B439" s="63" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C439" s="62" t="s">
         <v>1173</v>
-      </c>
-      <c r="C439" s="62" t="s">
-        <v>1174</v>
       </c>
       <c r="D439" s="65" t="s">
         <v>471</v>
@@ -12100,10 +12097,10 @@
         <v>125</v>
       </c>
       <c r="B440" s="63" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="C440" s="62" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="D440" s="65" t="s">
         <v>528</v>
@@ -12114,10 +12111,10 @@
         <v>125</v>
       </c>
       <c r="B441" s="63" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="C441" s="70" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="D441" s="65"/>
     </row>
@@ -12126,10 +12123,10 @@
         <v>125</v>
       </c>
       <c r="B442" s="63" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="C442" s="72" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="D442" s="65" t="s">
         <v>479</v>
@@ -12140,10 +12137,10 @@
         <v>125</v>
       </c>
       <c r="B443" s="63" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C443" s="69" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="E443" s="65" t="s">
         <v>932</v>
@@ -12154,10 +12151,10 @@
         <v>125</v>
       </c>
       <c r="B444" s="63" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C444" s="70" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="D444" s="65"/>
     </row>
@@ -12166,7 +12163,7 @@
         <v>125</v>
       </c>
       <c r="B445" s="63" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="C445" s="72" t="s">
         <v>473</v>
@@ -12180,10 +12177,10 @@
         <v>125</v>
       </c>
       <c r="B446" s="63" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="C446" s="72" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="D446" s="65" t="s">
         <v>477</v>
@@ -12194,10 +12191,10 @@
         <v>125</v>
       </c>
       <c r="B447" s="63" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="C447" s="72" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="D447" s="65" t="s">
         <v>479</v>
@@ -12208,10 +12205,10 @@
         <v>125</v>
       </c>
       <c r="B448" s="63" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C448" s="63" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="D448" s="65" t="s">
         <v>479</v>
@@ -12222,10 +12219,10 @@
         <v>125</v>
       </c>
       <c r="B449" s="63" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="C449" s="69" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="E449" s="65" t="s">
         <v>932</v>
@@ -13152,7 +13149,7 @@
     </row>
     <row r="38" spans="1:7" ht="31.5">
       <c r="C38" s="16" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D38" s="50" t="s">
         <v>438</v>

</xml_diff>